<commit_message>
feat: add package v1.1.2 for D2.35
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -448,7 +448,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,7 +480,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>V1.1.0</v>
+        <v>COVAC</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +488,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.35.1-bca7d7b</v>
+        <v>TRACKER</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>20210303T015519</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_V1.1.0_DHIS2.35.1-bca7d7b_20210303T015519</v>
+        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.35.1-bca7d7b_20210318T015424</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +581,10 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Given name</v>
+        <v>sB1IHYu2xQT</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>TfdH5KvFmMy</v>
+        <v>sB1IHYu2xQT</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
@@ -598,10 +598,10 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Family name</v>
+        <v>ENRjVGxVL6l</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>aW66s2QSosT</v>
+        <v>ENRjVGxVL6l</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
@@ -615,10 +615,10 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Sex</v>
+        <v>oindugucx72</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>CklPZdOd6H1</v>
+        <v>oindugucx72</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
@@ -646,13 +646,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zTWSj3Lg5KP</v>
+        <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Date of birth (age)</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>mAWcalQYYyk</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -669,7 +669,7 @@
         <v>Mobile phone number</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>ciCR6BBvIT4</v>
+        <v>fctSQp5nAYl</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -683,10 +683,10 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Address (current)</v>
+        <v>Xhdn49gUd52</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>VCtm2pySeEV</v>
+        <v>Xhdn49gUd52</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
@@ -780,7 +780,7 @@
         <v>COVAC - AEFIs present</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>AEFIs_present</v>
+        <v>COVAC_AEFIs_present</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>Are there any adverse events present after receiving the immunization?</v>
@@ -1197,7 +1197,7 @@
         <v>totalDoses</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v xml:space="preserve">Total doses required for this vaccine product </v>
+        <v>Total doses required for this vaccine product</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>default</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
       <c r="C23" s="5" t="str">
         <v>COVAC_vaccine_manufacturer</v>
@@ -1337,7 +1337,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - Dose Number</v>
       </c>
     </row>
     <row r="4">
@@ -1345,7 +1345,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC - Dose Number</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="5">
@@ -1353,7 +1353,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="6">
@@ -1361,7 +1361,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC- Batch Number</v>
+        <v>COVAC - Pregnancy</v>
       </c>
     </row>
     <row r="7">
@@ -1369,7 +1369,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="8">
@@ -1377,7 +1377,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="9">
@@ -1385,7 +1385,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVAC - Malignancy</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="10">
@@ -1393,7 +1393,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAC - Pregnancy</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="11">
@@ -1401,7 +1401,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="12">
@@ -1409,7 +1409,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="13">
@@ -1417,7 +1417,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="14">
@@ -1425,7 +1425,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="15">
@@ -1433,7 +1433,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC- Batch Number</v>
       </c>
     </row>
     <row r="16">
@@ -1441,7 +1441,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Cardiovascular Disease</v>
+        <v>COVAC - Malignancy</v>
       </c>
     </row>
     <row r="17">
@@ -1449,7 +1449,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="18">
@@ -1457,7 +1457,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
     <row r="19">
@@ -1465,7 +1465,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="20">
@@ -1473,7 +1473,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Chronic Lung Disease</v>
+        <v>COVAC - Cardiovascular Disease</v>
       </c>
     </row>
     <row r="21">
@@ -1481,7 +1481,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="22">
@@ -1489,7 +1489,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Chronic Lung Disease</v>
       </c>
     </row>
     <row r="23">
@@ -1497,7 +1497,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="24">
@@ -1758,7 +1758,7 @@
         <v>kgDmgTYZICP</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>1st Trimester (1-12 weeks); 2nd Trimester (13-28 weeks); 3rd Trimester (20-40 weeks)</v>
+        <v>1st Trimester (1-12 weeks); 2nd Trimester (13-28 weeks); 3rd Trimester (29-40 weeks)</v>
       </c>
     </row>
     <row r="6">
@@ -1805,13 +1805,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Sex</v>
+        <v>Sex</v>
       </c>
       <c r="B9" s="5" t="str">
         <v/>
       </c>
       <c r="C9" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>Female; Male</v>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Yes/No/Unknown</v>
+        <v>Yes/No/Unknown</v>
       </c>
       <c r="B10" s="4" t="str">
         <v/>
       </c>
       <c r="C10" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>Yes; No; Unknown</v>
@@ -1956,7 +1956,7 @@
         <v>Q3obJT1MXov</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>3rd Trimester (20-40 weeks)</v>
+        <v>3rd Trimester (29-40 weeks)</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>3trimester</v>
@@ -2089,19 +2089,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>AZK4rjJCss5</v>
+        <v>FKKrOBBFgs1</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>FEMALE</v>
+        <v>Female</v>
       </c>
       <c r="D15" s="5" t="str">
         <v/>
       </c>
       <c r="E15" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
     </row>
     <row r="16">
@@ -2191,19 +2191,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>UrUdMteQzlT</v>
+        <v>Ii4IxCLWEFn</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Male</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>MALE</v>
+        <v>Male</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
       </c>
       <c r="E21" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
     </row>
     <row r="22">
@@ -2242,19 +2242,19 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>PLlPgcfbL1D</v>
+        <v>R98tI2c6rF5</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>No</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>NO</v>
+        <v>No</v>
       </c>
       <c r="D24" s="4" t="str">
         <v/>
       </c>
       <c r="E24" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
     <row r="25">
@@ -2514,19 +2514,19 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>TKD1XJ4ZhMO</v>
+        <v>pqxvAQU1z9W</v>
       </c>
       <c r="B40" s="4" t="str">
         <v>Unknown</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>UNKNOWN</v>
+        <v>Unknown</v>
       </c>
       <c r="D40" s="4" t="str">
         <v/>
       </c>
       <c r="E40" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
     <row r="41">
@@ -2548,19 +2548,19 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>CvivP1rh4ii</v>
+        <v>x9yVKkv9koc</v>
       </c>
       <c r="B42" s="4" t="str">
         <v>Yes</v>
       </c>
       <c r="C42" s="4" t="str">
-        <v>YES</v>
+        <v>Yes</v>
       </c>
       <c r="D42" s="4" t="str">
         <v/>
       </c>
       <c r="E42" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
   </sheetData>
@@ -3454,21 +3454,21 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVAC - At least one underlying condition</v>
+        <v>COVAC - People with completed vaccination schedule</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v/>
+        <v>COVAC - People with completed vaccination schedule</v>
       </c>
       <c r="C2" s="4" t="str">
         <v/>
       </c>
       <c r="D2" s="4" t="str">
-        <v>gNsB9zivLTy</v>
+        <v>TWG0cq8P539</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVAC - Complete vaccination uptake</v>
+        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
       </c>
       <c r="B3" s="5" t="str">
         <v/>
@@ -3477,26 +3477,26 @@
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>aUjo2Myd25f</v>
+        <v>wHd33PaphEC</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
+        <v>COVAC - At least one underlying condition</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>TEST TEST</v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
       </c>
       <c r="D4" s="4" t="str">
-        <v>vmNUVdhuxN7</v>
+        <v>gNsB9zivLTy</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVAC - Drop-out from COV-1 to COV-c</v>
+        <v>COVAC - Underlying conditions</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
@@ -3505,7 +3505,7 @@
         <v/>
       </c>
       <c r="D5" s="5" t="str">
-        <v>Hbs3xGj7XoN</v>
+        <v>vFkbMQiABfj</v>
       </c>
     </row>
     <row r="6">
@@ -3524,7 +3524,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
+        <v>COVAC - Complete vaccination uptake</v>
       </c>
       <c r="B7" s="5" t="str">
         <v/>
@@ -3533,26 +3533,26 @@
         <v/>
       </c>
       <c r="D7" s="5" t="str">
-        <v>wHd33PaphEC</v>
+        <v>aUjo2Myd25f</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVAC - People with completed vaccination schedule</v>
+        <v>COVAC - Vaccine uptake by sex</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - People with completed vaccination schedule</v>
+        <v/>
       </c>
       <c r="C8" s="4" t="str">
         <v/>
       </c>
       <c r="D8" s="4" t="str">
-        <v>TWG0cq8P539</v>
+        <v>KV7fffdXnlY</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Underlying conditions</v>
+        <v>COVAC - Vaccine uptake by age group</v>
       </c>
       <c r="B9" s="5" t="str">
         <v/>
@@ -3561,12 +3561,12 @@
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>vFkbMQiABfj</v>
+        <v>BWlYGFBDbO2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Vaccine uptake by age group</v>
+        <v>COVAC - Vaccine uptake, last month</v>
       </c>
       <c r="B10" s="4" t="str">
         <v/>
@@ -3575,12 +3575,12 @@
         <v/>
       </c>
       <c r="D10" s="4" t="str">
-        <v>BWlYGFBDbO2</v>
+        <v>MzSAvoJ0vLr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVAC - Vaccine uptake by sex</v>
+        <v>COVAC - Drop-out from COV-1 to COV-c</v>
       </c>
       <c r="B11" s="5" t="str">
         <v/>
@@ -3589,21 +3589,21 @@
         <v/>
       </c>
       <c r="D11" s="5" t="str">
-        <v>KV7fffdXnlY</v>
+        <v>Hbs3xGj7XoN</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>COVAC - Vaccine uptake, last month</v>
+        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v/>
+        <v>TEST TEST</v>
       </c>
       <c r="C12" s="4" t="str">
         <v/>
       </c>
       <c r="D12" s="4" t="str">
-        <v>MzSAvoJ0vLr</v>
+        <v>vmNUVdhuxN7</v>
       </c>
     </row>
   </sheetData>
@@ -3910,7 +3910,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -3949,14 +3949,6 @@
       </c>
       <c r="B4" s="4" t="str">
         <v>qb8PkSObwqh</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Person</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>loHxNJH4IvV</v>
       </c>
     </row>
   </sheetData>
@@ -4003,14 +3995,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="112.7109375" customWidth="1"/>
+    <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4034,75 +4026,75 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Address (current)</v>
+        <v>Area Urban Rural</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v/>
+        <v>area_urban_rural</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v xml:space="preserve">Current home address of the patient/case </v>
+        <v>Whether client lives in an urban or rural setting</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
       </c>
       <c r="E2" s="4" t="str">
-        <v>VCtm2pySeEV</v>
+        <v>YCqoNJZKvAG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Area Urban Rural</v>
+        <v>COVID - Occupation</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>area_urban_rural</v>
+        <v>occupation</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Whether client lives in an urban or rural setting</v>
+        <v>Client occupation from the pre-defined list</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>YCqoNJZKvAG</v>
+        <v>LY2bDXpNvS7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID - Occupation</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>occupation</v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Client occupation from the pre-defined list</v>
+        <v/>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>LY2bDXpNvS7</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Date of birth (age)</v>
+        <v>Mobile phone number</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Date of birth plus calculated age</v>
+        <v/>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>mAWcalQYYyk</v>
+        <v>fctSQp5nAYl</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>National ID</v>
       </c>
       <c r="B6" s="4" t="str">
         <v/>
@@ -4114,108 +4106,23 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>Ewi7FUfcHAD</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Family name</v>
+        <v>Unique System Identifier (EPI)</v>
       </c>
       <c r="B7" s="5" t="str">
         <v/>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Family name of the patient</v>
+        <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>aW66s2QSosT</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="str">
-        <v>Given name</v>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>The name of the patient or initials</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>TfdH5KvFmMy</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="str">
-        <v>Mobile phone number</v>
-      </c>
-      <c r="B9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>ciCR6BBvIT4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="str">
-        <v>National ID</v>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVAC - Sex</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v>covac_patinfo_sex</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>Sex of Person</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>CklPZdOd6H1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>Unique System Identifier (EPI)</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>System-generated unique ID following pattern: CURRENT_DATE(yyyy-MM-dd) followed by a sequential number (#####)</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4258,7 +4165,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-02</v>
+        <v>2021-03-16</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>
@@ -4297,7 +4204,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>a1jCssI2LkW</v>
@@ -4338,7 +4245,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>Vaccination information</v>
@@ -4349,7 +4256,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Vaccination information</v>
@@ -4360,7 +4267,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Vaccination information</v>
@@ -4371,7 +4278,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Vaccination information</v>
@@ -4382,7 +4289,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Vaccination information</v>
@@ -4393,7 +4300,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B7" s="5" t="str">
         <v>Vaccination information</v>
@@ -4404,7 +4311,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B8" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4415,7 +4322,7 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4426,7 +4333,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B10" s="4" t="str">
         <v>Pre-immunization Questions</v>
@@ -4437,7 +4344,7 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B11" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4448,7 +4355,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4459,7 +4366,7 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B13" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4470,7 +4377,7 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B14" s="4" t="str">
         <v>Pre-immunization Questions</v>
@@ -4481,7 +4388,7 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4492,7 +4399,7 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B16" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4503,7 +4410,7 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B17" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4514,7 +4421,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B18" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4525,7 +4432,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B19" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4536,18 +4443,18 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B20" s="4" t="str">
         <v>Vaccination information</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4558,7 +4465,7 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B22" s="4" t="str">
         <v>Vaccination information</v>
@@ -4569,7 +4476,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Vaccination information</v>
@@ -4580,7 +4487,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>Vaccination information</v>
@@ -4953,7 +4860,7 @@
         <v>kNzRGpiCvg4</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v xml:space="preserve">Doses given </v>
+        <v>Doses given</v>
       </c>
       <c r="C14" s="4" t="str">
         <v xml:space="preserve">1st, 2nd, 3rd, booster dose - Number of doses - </v>
@@ -4979,7 +4886,7 @@
         <v>AXweWKC4B3L</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v xml:space="preserve">Number of people receiving a first dose </v>
+        <v>Number of people receiving a first dose</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>First dose - Number of people</v>
@@ -5213,7 +5120,7 @@
         <v>zr25iLoCE4g</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v xml:space="preserve">Number of people receiving a second, third or booster dose </v>
+        <v>Number of people receiving a second, third or booster dose</v>
       </c>
       <c r="C24" s="4" t="str">
         <v>2nd, 3rd, booster dose - Number of people</v>
@@ -5242,7 +5149,7 @@
         <v xml:space="preserve">Number of people receiving a second, third or booster dose  (Male) </v>
       </c>
       <c r="C25" s="5" t="str">
-        <v xml:space="preserve">2nd, 3rd, booster dose - Number of males </v>
+        <v>2nd, 3rd, booster dose - Number of males</v>
       </c>
       <c r="D25" s="5" t="str">
         <v>COV-2 (Male)</v>
@@ -5372,7 +5279,7 @@
         <v xml:space="preserve">Number of people receiving a second, third or booster dose (Female) </v>
       </c>
       <c r="C30" s="4" t="str">
-        <v xml:space="preserve">2nd, 3rd, booster dose - Number of females </v>
+        <v>2nd, 3rd, booster dose - Number of females</v>
       </c>
       <c r="D30" s="4" t="str">
         <v>COV-2 (Female)</v>
@@ -5840,7 +5747,7 @@
         <v>ZZZNumber of doses given</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v xml:space="preserve">ZZZ1st, 2nd, 3rd, booster dose - Number of people </v>
+        <v>ZZZ1st, 2nd, 3rd, booster dose - Number of people</v>
       </c>
       <c r="D48" s="4" t="str">
         <v>ZZZCOV-n</v>
@@ -5863,7 +5770,7 @@
         <v>BEw3zmRnGo4</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v xml:space="preserve">ZZZNumber of people (Female) receiving a second, third or booster dose </v>
+        <v>ZZZNumber of people (Female) receiving a second, third or booster dose</v>
       </c>
       <c r="C49" s="5" t="str">
         <v>ZZZ2nd, 3rd, booster dose - Number of females</v>
@@ -5889,7 +5796,7 @@
         <v>IXW8ahBF3Pl</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v xml:space="preserve">ZZZNumber of people (Male) receiving a second, third or booster dose </v>
+        <v>ZZZNumber of people (Male) receiving a second, third or booster dose</v>
       </c>
       <c r="C50" s="4" t="str">
         <v>ZZZ2nd, 3rd, booster dose - Number of males</v>
@@ -5941,10 +5848,10 @@
         <v>sYIBsws6qUG</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v xml:space="preserve">zzzNumber of people receiving a second, third or booster dose </v>
+        <v>zzzNumber of people receiving a second, third or booster dose</v>
       </c>
       <c r="C52" s="4" t="str">
-        <v xml:space="preserve">zzz2nd, 3rd, booster dose - Number of people </v>
+        <v>zzz2nd, 3rd, booster dose - Number of people</v>
       </c>
       <c r="D52" s="4" t="str">
         <v xml:space="preserve">zzzCOV-2 </v>
@@ -6046,7 +5953,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -6335,7 +6242,7 @@
         <v>oPUB5us9T8e</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v xml:space="preserve">Calculate age </v>
+        <v>Calculate age</v>
       </c>
       <c r="C17" s="5" t="str">
         <v/>
@@ -6400,13 +6307,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>HdOtRsvVzgY</v>
+        <v>R1bzqObecyQ</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Hide Trimester if nor pregnant</v>
+        <v>Hide Suggested date for next dose if vaccine product has no more doses</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v/>
+        <v>All vaccine types with two doses, after they receive one does, the "next dose date" will be hidden.</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
@@ -6417,10 +6324,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>I0FZ4YQgxfD</v>
+        <v>HdOtRsvVzgY</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>Hide underlying conditions if none</v>
+        <v>Hide Trimester if nor pregnant</v>
       </c>
       <c r="C22" s="4" t="str">
         <v/>
@@ -6434,10 +6341,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>TRR2ODBsnkN</v>
+        <v>I0FZ4YQgxfD</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>If Age is under 16, then warn that BioNTech/Pfizer is recommended for ages 16 and up</v>
+        <v>Hide underlying conditions if none</v>
       </c>
       <c r="C23" s="5" t="str">
         <v/>
@@ -6451,10 +6358,10 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>e0WJRMhSrZy</v>
+        <v>TRR2ODBsnkN</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>If Age is under 18, then warn that AstraZeneca is recommended for ages 18 and up</v>
+        <v>If Age is under 16, then warn that BioNTech/Pfizer is recommended for ages 16 and up</v>
       </c>
       <c r="C24" s="4" t="str">
         <v/>
@@ -6468,10 +6375,10 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>xydE4Vcj6xU</v>
+        <v>e0WJRMhSrZy</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>If Age is under 18, then warn that Gamaleya is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that AstraZeneca is recommended for ages 18 and up</v>
       </c>
       <c r="C25" s="5" t="str">
         <v/>
@@ -6485,10 +6392,10 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>ppbeGorruVj</v>
+        <v>xydE4Vcj6xU</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>If Age is under 18, then warn that Moderna is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that Gamaleya is recommended for ages 18 and up</v>
       </c>
       <c r="C26" s="4" t="str">
         <v/>
@@ -6502,10 +6409,10 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>xeInMQrA5Mo</v>
+        <v>ppbeGorruVj</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>If Age is under 18, then warn that Sinopharm is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that Moderna is recommended for ages 18 and up</v>
       </c>
       <c r="C27" s="5" t="str">
         <v/>
@@ -6519,10 +6426,10 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>jNtY9t6b120</v>
+        <v>xeInMQrA5Mo</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>if client has a history of cardiovascular disease assign value to current event</v>
+        <v>If Age is under 18, then warn that Sinopharm is recommended for ages 18 and up</v>
       </c>
       <c r="C28" s="4" t="str">
         <v/>
@@ -6536,10 +6443,10 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>j16AULHWXur</v>
+        <v>jNtY9t6b120</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>If client has a history of Cardiovascular disease show it on indicator panel</v>
+        <v>if client has a history of cardiovascular disease assign value to current event</v>
       </c>
       <c r="C29" s="5" t="str">
         <v/>
@@ -6553,10 +6460,10 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>gmBh14b7tYb</v>
+        <v>j16AULHWXur</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>If client has a history of Chronic lung disease show it on indicator panel</v>
+        <v>If client has a history of Cardiovascular disease show it on indicator panel</v>
       </c>
       <c r="C30" s="4" t="str">
         <v/>
@@ -6570,10 +6477,10 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>i0YmXeSnrqn</v>
+        <v>gmBh14b7tYb</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>if client has a history of Chronic lung disease, add value to current event</v>
+        <v>If client has a history of Chronic lung disease show it on indicator panel</v>
       </c>
       <c r="C31" s="5" t="str">
         <v/>
@@ -6587,10 +6494,10 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>KGBdMuY2ASs</v>
+        <v>i0YmXeSnrqn</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>if client has a history of Diabetes assign value to current event</v>
+        <v>if client has a history of Chronic lung disease, add value to current event</v>
       </c>
       <c r="C32" s="4" t="str">
         <v/>
@@ -6604,10 +6511,10 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>r9NQ2R4eFIO</v>
+        <v>KGBdMuY2ASs</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>If client has a history of Diabetes show it on indicator panel</v>
+        <v>if client has a history of Diabetes assign value to current event</v>
       </c>
       <c r="C33" s="5" t="str">
         <v/>
@@ -6621,10 +6528,10 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>i5tOyWRc3S1</v>
+        <v>r9NQ2R4eFIO</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>if client has a history of immunodeficiency assign value to current event</v>
+        <v>If client has a history of Diabetes show it on indicator panel</v>
       </c>
       <c r="C34" s="4" t="str">
         <v/>
@@ -6638,10 +6545,10 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>ucrvgwsRCim</v>
+        <v>i5tOyWRc3S1</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>If client has a history of immunodeficiency show it on indicator panel</v>
+        <v>if client has a history of immunodeficiency assign value to current event</v>
       </c>
       <c r="C35" s="5" t="str">
         <v/>
@@ -6655,10 +6562,10 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>K9Vjkz1xOw1</v>
+        <v>ucrvgwsRCim</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>if client has a history of malignancy assign value to current event</v>
+        <v>If client has a history of immunodeficiency show it on indicator panel</v>
       </c>
       <c r="C36" s="4" t="str">
         <v/>
@@ -6672,10 +6579,10 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>SDfSLD0WFOL</v>
+        <v>K9Vjkz1xOw1</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>if client has a history of malignancy show it on indicator panel</v>
+        <v>if client has a history of malignancy assign value to current event</v>
       </c>
       <c r="C37" s="5" t="str">
         <v/>
@@ -6689,10 +6596,10 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>OdSVYvgu6G2</v>
+        <v>SDfSLD0WFOL</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>if client has a history of neurological deficiency assign value to current event</v>
+        <v>if client has a history of malignancy show it on indicator panel</v>
       </c>
       <c r="C38" s="4" t="str">
         <v/>
@@ -6706,10 +6613,10 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>vqQMyfw3i3u</v>
+        <v>OdSVYvgu6G2</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>If client has a history of Neurological disease show it on indicator panel</v>
+        <v>if client has a history of neurological deficiency assign value to current event</v>
       </c>
       <c r="C39" s="5" t="str">
         <v/>
@@ -6723,10 +6630,10 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>QEq5oRr4UEw</v>
+        <v>vqQMyfw3i3u</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>if client has a history of Other assign value to current event</v>
+        <v>If client has a history of Neurological disease show it on indicator panel</v>
       </c>
       <c r="C40" s="4" t="str">
         <v/>
@@ -6740,10 +6647,10 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="str">
-        <v>ParDbFN1amU</v>
+        <v>QEq5oRr4UEw</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>If client has a history of OTHER disease show it on indicator panel</v>
+        <v>if client has a history of Other assign value to current event</v>
       </c>
       <c r="C41" s="5" t="str">
         <v/>
@@ -6757,10 +6664,10 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>l8opvp32VAd</v>
+        <v>ParDbFN1amU</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>if client has a history of Renal disease assign value to current event</v>
+        <v>If client has a history of OTHER disease show it on indicator panel</v>
       </c>
       <c r="C42" s="4" t="str">
         <v/>
@@ -6774,10 +6681,10 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="str">
-        <v>qrIXRSq77JN</v>
+        <v>l8opvp32VAd</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>If client has a history of Renal Disease show it on indicator panel</v>
+        <v>if client has a history of Renal disease assign value to current event</v>
       </c>
       <c r="C43" s="5" t="str">
         <v/>
@@ -6791,13 +6698,13 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
-        <v>GtxjhHBQdLQ</v>
+        <v>qrIXRSq77JN</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>If patient has had covid, assign value to data element of current event</v>
+        <v>If client has a history of Renal Disease show it on indicator panel</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>Rule transfers date of remission and if person has previously had covid</v>
+        <v/>
       </c>
       <c r="D44" s="4" t="str">
         <v/>
@@ -6808,10 +6715,10 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
-        <v>AmgPexdbztQ</v>
+        <v>GtxjhHBQdLQ</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>If patient has had underlying diseases, transfer that value to following stage</v>
+        <v>If patient has had covid, assign value to data element of current event</v>
       </c>
       <c r="C45" s="5" t="str">
         <v>Rule transfers date of remission and if person has previously had covid</v>
@@ -6825,10 +6732,10 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
-        <v>XTLv9YqOtNX</v>
+        <v>AmgPexdbztQ</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>If previous vaccine is differente than current vaccine, show warning.</v>
+        <v>If patient has had underlying diseases, transfer that value to following stage</v>
       </c>
       <c r="C46" s="4" t="str">
         <v/>
@@ -6842,10 +6749,10 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
-        <v>vd1vZsjDft4</v>
+        <v>XTLv9YqOtNX</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>If previous vaccine is same as current vaccine, hide explanation field</v>
+        <v>If previous vaccine is differente than current vaccine, show warning.</v>
       </c>
       <c r="C47" s="5" t="str">
         <v/>
@@ -6859,10 +6766,10 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
-        <v>A6Oy09dbQwn</v>
+        <v>vd1vZsjDft4</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>if there was an allergic reaction after the first dose, show warning "conduct AEFI Investigation"</v>
+        <v>If previous vaccine is same as current vaccine, hide explanation field</v>
       </c>
       <c r="C48" s="4" t="str">
         <v/>
@@ -6876,13 +6783,13 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="str">
-        <v>PJjKiFrvfuN</v>
+        <v>A6Oy09dbQwn</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>If this is the second dose, mark it as "last dose" for all vaccine products</v>
+        <v>if there was an allergic reaction after the first dose, show warning "conduct AEFI Investigation"</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>It selects the "last dose" option, it assumes that all products have two doses as the complete schedule.</v>
+        <v/>
       </c>
       <c r="D49" s="5" t="str">
         <v/>
@@ -6893,13 +6800,13 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
-        <v>SkBUqyO9zG0</v>
+        <v>PJjKiFrvfuN</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>Last dose - complete programme</v>
+        <v>If this is the second dose, mark it as "last dose" for all vaccine products</v>
       </c>
       <c r="C50" s="4" t="str">
-        <v/>
+        <v>It selects the "last dose" option, it assumes that all products have two doses as the complete schedule.</v>
       </c>
       <c r="D50" s="4" t="str">
         <v/>
@@ -6910,10 +6817,10 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
-        <v>W0YQaz1qRJb</v>
+        <v>SkBUqyO9zG0</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>Send notification if overdue</v>
+        <v>Last dose - complete programme</v>
       </c>
       <c r="C51" s="5" t="str">
         <v/>
@@ -6927,10 +6834,10 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="str">
-        <v>nU9WWRKt7PL</v>
+        <v>W0YQaz1qRJb</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v>Show vaccine type from previous vaccination event</v>
+        <v>Send notification if overdue</v>
       </c>
       <c r="C52" s="4" t="str">
         <v/>
@@ -6944,10 +6851,10 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="str">
-        <v>LO6XtDyCbya</v>
+        <v>nU9WWRKt7PL</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>Show warning if person has had covid within 90 days of vaccination date</v>
+        <v>Show vaccine type from previous vaccination event</v>
       </c>
       <c r="C53" s="5" t="str">
         <v/>
@@ -6961,13 +6868,13 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="str">
-        <v>biYqhZM5HXe</v>
+        <v>LO6XtDyCbya</v>
       </c>
       <c r="B54" s="4" t="str">
-        <v>Show warning if the client is a health worker</v>
+        <v>Show warning if person has had covid within 90 days of vaccination date</v>
       </c>
       <c r="C54" s="4" t="str">
-        <v>If the client is a health worker, show a warning in the top bar</v>
+        <v/>
       </c>
       <c r="D54" s="4" t="str">
         <v/>
@@ -6978,18 +6885,35 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
+        <v>biYqhZM5HXe</v>
+      </c>
+      <c r="B55" s="5" t="str">
+        <v>Show warning if the client is a health worker</v>
+      </c>
+      <c r="C55" s="5" t="str">
+        <v>If the client is a health worker, show a warning in the top bar</v>
+      </c>
+      <c r="D55" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E55" s="5" t="str">
+        <v>yDuAzyqYABS</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="str">
         <v>hdPflHqZKO3</v>
       </c>
-      <c r="B55" s="5" t="str">
+      <c r="B56" s="4" t="str">
         <v>Show warning: If first dose, then hide "last dose" DE</v>
       </c>
-      <c r="C55" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D55" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E55" s="5" t="str">
+      <c r="C56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E56" s="4" t="str">
         <v>yDuAzyqYABS</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add package v1.1.2 for D2.34
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -448,7 +448,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,7 +480,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>V1.1.0</v>
+        <v>COVAC</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +488,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.34.3-80c86cc</v>
+        <v>TRACKER</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>20210303T014351</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_V1.1.0_DHIS2.34.3-80c86cc_20210303T014351</v>
+        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.34.3-80c86cc_20210318T014413</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +581,10 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Given name</v>
+        <v>sB1IHYu2xQT</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>TfdH5KvFmMy</v>
+        <v>sB1IHYu2xQT</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
@@ -598,10 +598,10 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Family name</v>
+        <v>ENRjVGxVL6l</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>aW66s2QSosT</v>
+        <v>ENRjVGxVL6l</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
@@ -615,10 +615,10 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Sex</v>
+        <v>oindugucx72</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>CklPZdOd6H1</v>
+        <v>oindugucx72</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
@@ -646,13 +646,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zTWSj3Lg5KP</v>
+        <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Date of birth (age)</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>mAWcalQYYyk</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -669,7 +669,7 @@
         <v>Mobile phone number</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>ciCR6BBvIT4</v>
+        <v>fctSQp5nAYl</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -683,10 +683,10 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Address (current)</v>
+        <v>Xhdn49gUd52</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>VCtm2pySeEV</v>
+        <v>Xhdn49gUd52</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
@@ -780,7 +780,7 @@
         <v>COVAC - AEFIs present</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>AEFIs_present</v>
+        <v>COVAC_AEFIs_present</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>Are there any adverse events present after receiving the immunization?</v>
@@ -1197,7 +1197,7 @@
         <v>totalDoses</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v xml:space="preserve">Total doses required for this vaccine product </v>
+        <v>Total doses required for this vaccine product</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>default</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
       <c r="C23" s="5" t="str">
         <v>COVAC_vaccine_manufacturer</v>
@@ -1329,7 +1329,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="3">
@@ -1337,7 +1337,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Underlying condition</v>
       </c>
     </row>
     <row r="4">
@@ -1345,7 +1345,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC- Batch Number</v>
       </c>
     </row>
     <row r="5">
@@ -1353,7 +1353,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Pregnancy</v>
       </c>
     </row>
     <row r="6">
@@ -1361,7 +1361,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC - Dose Expiry Date</v>
       </c>
     </row>
     <row r="7">
@@ -1369,7 +1369,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - Underlying condition</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="8">
@@ -1377,7 +1377,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC - Dose Number</v>
       </c>
     </row>
     <row r="9">
@@ -1385,7 +1385,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVAC- Batch Number</v>
+        <v>COVAC - Cardiovascular Disease</v>
       </c>
     </row>
     <row r="10">
@@ -1393,7 +1393,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC - Chronic Lung Disease</v>
       </c>
     </row>
     <row r="11">
@@ -1401,7 +1401,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="12">
@@ -1409,7 +1409,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC - Pregnancy</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="13">
@@ -1417,7 +1417,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC - Dose Expiry Date</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
     <row r="14">
@@ -1425,7 +1425,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="15">
@@ -1433,7 +1433,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="16">
@@ -1441,7 +1441,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="17">
@@ -1449,7 +1449,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="18">
@@ -1457,7 +1457,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC - Malignancy</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="19">
@@ -1465,7 +1465,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC - Dose Number</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="20">
@@ -1473,7 +1473,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Cardiovascular Disease</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="21">
@@ -1481,7 +1481,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Chronic Lung Disease</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="22">
@@ -1489,7 +1489,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="23">
@@ -1497,7 +1497,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC - Malignancy</v>
       </c>
     </row>
     <row r="24">
@@ -1505,7 +1505,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1758,7 @@
         <v>kgDmgTYZICP</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>1st Trimester (1-12 weeks); 2nd Trimester (13-28 weeks); 3rd Trimester (20-40 weeks)</v>
+        <v>1st Trimester (1-12 weeks); 2nd Trimester (13-28 weeks); 3rd Trimester (29-40 weeks)</v>
       </c>
     </row>
     <row r="6">
@@ -1805,13 +1805,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Sex</v>
+        <v>Sex</v>
       </c>
       <c r="B9" s="5" t="str">
         <v/>
       </c>
       <c r="C9" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>Female; Male</v>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Yes/No/Unknown</v>
+        <v>Yes/No/Unknown</v>
       </c>
       <c r="B10" s="4" t="str">
         <v/>
       </c>
       <c r="C10" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>Yes; No; Unknown</v>
@@ -1956,7 +1956,7 @@
         <v>Q3obJT1MXov</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>3rd Trimester (20-40 weeks)</v>
+        <v>3rd Trimester (29-40 weeks)</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>3trimester</v>
@@ -2089,19 +2089,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>AZK4rjJCss5</v>
+        <v>FKKrOBBFgs1</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>FEMALE</v>
+        <v>Female</v>
       </c>
       <c r="D15" s="5" t="str">
         <v/>
       </c>
       <c r="E15" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
     </row>
     <row r="16">
@@ -2191,19 +2191,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>UrUdMteQzlT</v>
+        <v>Ii4IxCLWEFn</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Male</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>MALE</v>
+        <v>Male</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
       </c>
       <c r="E21" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
     </row>
     <row r="22">
@@ -2242,19 +2242,19 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>PLlPgcfbL1D</v>
+        <v>R98tI2c6rF5</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>No</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>NO</v>
+        <v>No</v>
       </c>
       <c r="D24" s="4" t="str">
         <v/>
       </c>
       <c r="E24" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
     <row r="25">
@@ -2514,19 +2514,19 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>TKD1XJ4ZhMO</v>
+        <v>pqxvAQU1z9W</v>
       </c>
       <c r="B40" s="4" t="str">
         <v>Unknown</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>UNKNOWN</v>
+        <v>Unknown</v>
       </c>
       <c r="D40" s="4" t="str">
         <v/>
       </c>
       <c r="E40" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
     <row r="41">
@@ -2548,19 +2548,19 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>CvivP1rh4ii</v>
+        <v>x9yVKkv9koc</v>
       </c>
       <c r="B42" s="4" t="str">
         <v>Yes</v>
       </c>
       <c r="C42" s="4" t="str">
-        <v>YES</v>
+        <v>Yes</v>
       </c>
       <c r="D42" s="4" t="str">
         <v/>
       </c>
       <c r="E42" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
   </sheetData>
@@ -3454,21 +3454,21 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVAC - At least one underlying condition</v>
+        <v>COVAC - People with completed vaccination schedule</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v/>
+        <v>COVAC - People with completed vaccination schedule</v>
       </c>
       <c r="C2" s="4" t="str">
         <v/>
       </c>
       <c r="D2" s="4" t="str">
-        <v>gNsB9zivLTy</v>
+        <v>TWG0cq8P539</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVAC - Complete vaccination uptake</v>
+        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
       </c>
       <c r="B3" s="5" t="str">
         <v/>
@@ -3477,26 +3477,26 @@
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>aUjo2Myd25f</v>
+        <v>wHd33PaphEC</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
+        <v>COVAC - At least one underlying condition</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>TEST TEST</v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
       </c>
       <c r="D4" s="4" t="str">
-        <v>vmNUVdhuxN7</v>
+        <v>gNsB9zivLTy</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVAC - Drop-out from COV-1 to COV-c</v>
+        <v>COVAC - Underlying conditions</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
@@ -3505,7 +3505,7 @@
         <v/>
       </c>
       <c r="D5" s="5" t="str">
-        <v>Hbs3xGj7XoN</v>
+        <v>vFkbMQiABfj</v>
       </c>
     </row>
     <row r="6">
@@ -3524,7 +3524,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
+        <v>COVAC - Complete vaccination uptake</v>
       </c>
       <c r="B7" s="5" t="str">
         <v/>
@@ -3533,26 +3533,26 @@
         <v/>
       </c>
       <c r="D7" s="5" t="str">
-        <v>wHd33PaphEC</v>
+        <v>aUjo2Myd25f</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVAC - People with completed vaccination schedule</v>
+        <v>COVAC - Vaccine uptake by sex</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - People with completed vaccination schedule</v>
+        <v/>
       </c>
       <c r="C8" s="4" t="str">
         <v/>
       </c>
       <c r="D8" s="4" t="str">
-        <v>TWG0cq8P539</v>
+        <v>KV7fffdXnlY</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Underlying conditions</v>
+        <v>COVAC - Vaccine uptake by age group</v>
       </c>
       <c r="B9" s="5" t="str">
         <v/>
@@ -3561,12 +3561,12 @@
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>vFkbMQiABfj</v>
+        <v>BWlYGFBDbO2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Vaccine uptake by age group</v>
+        <v>COVAC - Vaccine uptake, last month</v>
       </c>
       <c r="B10" s="4" t="str">
         <v/>
@@ -3575,12 +3575,12 @@
         <v/>
       </c>
       <c r="D10" s="4" t="str">
-        <v>BWlYGFBDbO2</v>
+        <v>MzSAvoJ0vLr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVAC - Vaccine uptake by sex</v>
+        <v>COVAC - Drop-out from COV-1 to COV-c</v>
       </c>
       <c r="B11" s="5" t="str">
         <v/>
@@ -3589,21 +3589,21 @@
         <v/>
       </c>
       <c r="D11" s="5" t="str">
-        <v>KV7fffdXnlY</v>
+        <v>Hbs3xGj7XoN</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>COVAC - Vaccine uptake, last month</v>
+        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v/>
+        <v>TEST TEST</v>
       </c>
       <c r="C12" s="4" t="str">
         <v/>
       </c>
       <c r="D12" s="4" t="str">
-        <v>MzSAvoJ0vLr</v>
+        <v>vmNUVdhuxN7</v>
       </c>
     </row>
   </sheetData>
@@ -3910,7 +3910,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -3949,14 +3949,6 @@
       </c>
       <c r="B4" s="4" t="str">
         <v>qb8PkSObwqh</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Person</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>loHxNJH4IvV</v>
       </c>
     </row>
   </sheetData>
@@ -4003,14 +3995,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="112.7109375" customWidth="1"/>
+    <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4034,75 +4026,75 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Address (current)</v>
+        <v>Area Urban Rural</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v/>
+        <v>area_urban_rural</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v xml:space="preserve">Current home address of the patient/case </v>
+        <v>Whether client lives in an urban or rural setting</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
       </c>
       <c r="E2" s="4" t="str">
-        <v>VCtm2pySeEV</v>
+        <v>YCqoNJZKvAG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Area Urban Rural</v>
+        <v>COVID - Occupation</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>area_urban_rural</v>
+        <v>occupation</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Whether client lives in an urban or rural setting</v>
+        <v>Client occupation from the pre-defined list</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>YCqoNJZKvAG</v>
+        <v>LY2bDXpNvS7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID - Occupation</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>occupation</v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Client occupation from the pre-defined list</v>
+        <v/>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>LY2bDXpNvS7</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Date of birth (age)</v>
+        <v>Mobile phone number</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Date of birth plus calculated age</v>
+        <v/>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>mAWcalQYYyk</v>
+        <v>fctSQp5nAYl</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>National ID</v>
       </c>
       <c r="B6" s="4" t="str">
         <v/>
@@ -4114,108 +4106,23 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>Ewi7FUfcHAD</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Family name</v>
+        <v>Unique System Identifier (EPI)</v>
       </c>
       <c r="B7" s="5" t="str">
         <v/>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Family name of the patient</v>
+        <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>aW66s2QSosT</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="str">
-        <v>Given name</v>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>The name of the patient or initials</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>TfdH5KvFmMy</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="str">
-        <v>Mobile phone number</v>
-      </c>
-      <c r="B9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>ciCR6BBvIT4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="str">
-        <v>National ID</v>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVAC - Sex</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v>covac_patinfo_sex</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>Sex of Person</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>CklPZdOd6H1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>Unique System Identifier (EPI)</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>System-generated unique ID following pattern: CURRENT_DATE(yyyy-MM-dd) followed by a sequential number (#####)</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4258,7 +4165,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-02</v>
+        <v>2021-03-16</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>
@@ -4297,7 +4204,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>a1jCssI2LkW</v>
@@ -4338,7 +4245,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>Vaccination information</v>
@@ -4349,7 +4256,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Vaccination information</v>
@@ -4360,7 +4267,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Vaccination information</v>
@@ -4371,7 +4278,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Vaccination information</v>
@@ -4382,7 +4289,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Vaccination information</v>
@@ -4393,7 +4300,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B7" s="5" t="str">
         <v>Vaccination information</v>
@@ -4404,7 +4311,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B8" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4415,7 +4322,7 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4426,7 +4333,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B10" s="4" t="str">
         <v>Pre-immunization Questions</v>
@@ -4437,7 +4344,7 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B11" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4448,7 +4355,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4459,7 +4366,7 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B13" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4470,7 +4377,7 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B14" s="4" t="str">
         <v>Pre-immunization Questions</v>
@@ -4481,7 +4388,7 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4492,7 +4399,7 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B16" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4503,7 +4410,7 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B17" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4514,7 +4421,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B18" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4525,7 +4432,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B19" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4536,18 +4443,18 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B20" s="4" t="str">
         <v>Vaccination information</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4558,7 +4465,7 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B22" s="4" t="str">
         <v>Vaccination information</v>
@@ -4569,7 +4476,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Vaccination information</v>
@@ -4580,7 +4487,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>Vaccination information</v>
@@ -4953,7 +4860,7 @@
         <v>kNzRGpiCvg4</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v xml:space="preserve">Doses given </v>
+        <v>Doses given</v>
       </c>
       <c r="C14" s="4" t="str">
         <v xml:space="preserve">1st, 2nd, 3rd, booster dose - Number of doses - </v>
@@ -4979,7 +4886,7 @@
         <v>AXweWKC4B3L</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v xml:space="preserve">Number of people receiving a first dose </v>
+        <v>Number of people receiving a first dose</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>First dose - Number of people</v>
@@ -5213,7 +5120,7 @@
         <v>zr25iLoCE4g</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v xml:space="preserve">Number of people receiving a second, third or booster dose </v>
+        <v>Number of people receiving a second, third or booster dose</v>
       </c>
       <c r="C24" s="4" t="str">
         <v>2nd, 3rd, booster dose - Number of people</v>
@@ -5242,7 +5149,7 @@
         <v xml:space="preserve">Number of people receiving a second, third or booster dose  (Male) </v>
       </c>
       <c r="C25" s="5" t="str">
-        <v xml:space="preserve">2nd, 3rd, booster dose - Number of males </v>
+        <v>2nd, 3rd, booster dose - Number of males</v>
       </c>
       <c r="D25" s="5" t="str">
         <v>COV-2 (Male)</v>
@@ -5372,7 +5279,7 @@
         <v xml:space="preserve">Number of people receiving a second, third or booster dose (Female) </v>
       </c>
       <c r="C30" s="4" t="str">
-        <v xml:space="preserve">2nd, 3rd, booster dose - Number of females </v>
+        <v>2nd, 3rd, booster dose - Number of females</v>
       </c>
       <c r="D30" s="4" t="str">
         <v>COV-2 (Female)</v>
@@ -5840,7 +5747,7 @@
         <v>ZZZNumber of doses given</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v xml:space="preserve">ZZZ1st, 2nd, 3rd, booster dose - Number of people </v>
+        <v>ZZZ1st, 2nd, 3rd, booster dose - Number of people</v>
       </c>
       <c r="D48" s="4" t="str">
         <v>ZZZCOV-n</v>
@@ -5863,7 +5770,7 @@
         <v>BEw3zmRnGo4</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v xml:space="preserve">ZZZNumber of people (Female) receiving a second, third or booster dose </v>
+        <v>ZZZNumber of people (Female) receiving a second, third or booster dose</v>
       </c>
       <c r="C49" s="5" t="str">
         <v>ZZZ2nd, 3rd, booster dose - Number of females</v>
@@ -5889,7 +5796,7 @@
         <v>IXW8ahBF3Pl</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v xml:space="preserve">ZZZNumber of people (Male) receiving a second, third or booster dose </v>
+        <v>ZZZNumber of people (Male) receiving a second, third or booster dose</v>
       </c>
       <c r="C50" s="4" t="str">
         <v>ZZZ2nd, 3rd, booster dose - Number of males</v>
@@ -5941,10 +5848,10 @@
         <v>sYIBsws6qUG</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v xml:space="preserve">zzzNumber of people receiving a second, third or booster dose </v>
+        <v>zzzNumber of people receiving a second, third or booster dose</v>
       </c>
       <c r="C52" s="4" t="str">
-        <v xml:space="preserve">zzz2nd, 3rd, booster dose - Number of people </v>
+        <v>zzz2nd, 3rd, booster dose - Number of people</v>
       </c>
       <c r="D52" s="4" t="str">
         <v xml:space="preserve">zzzCOV-2 </v>
@@ -6046,7 +5953,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -6335,7 +6242,7 @@
         <v>oPUB5us9T8e</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v xml:space="preserve">Calculate age </v>
+        <v>Calculate age</v>
       </c>
       <c r="C17" s="5" t="str">
         <v/>
@@ -6400,13 +6307,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>HdOtRsvVzgY</v>
+        <v>R1bzqObecyQ</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Hide Trimester if nor pregnant</v>
+        <v>Hide Suggested date for next dose if vaccine product has no more doses</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v/>
+        <v>All vaccine types with two doses, after they receive one does, the "next dose date" will be hidden.</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
@@ -6417,10 +6324,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>I0FZ4YQgxfD</v>
+        <v>HdOtRsvVzgY</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>Hide underlying conditions if none</v>
+        <v>Hide Trimester if nor pregnant</v>
       </c>
       <c r="C22" s="4" t="str">
         <v/>
@@ -6434,10 +6341,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>TRR2ODBsnkN</v>
+        <v>I0FZ4YQgxfD</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>If Age is under 16, then warn that BioNTech/Pfizer is recommended for ages 16 and up</v>
+        <v>Hide underlying conditions if none</v>
       </c>
       <c r="C23" s="5" t="str">
         <v/>
@@ -6451,10 +6358,10 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>e0WJRMhSrZy</v>
+        <v>TRR2ODBsnkN</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>If Age is under 18, then warn that AstraZeneca is recommended for ages 18 and up</v>
+        <v>If Age is under 16, then warn that BioNTech/Pfizer is recommended for ages 16 and up</v>
       </c>
       <c r="C24" s="4" t="str">
         <v/>
@@ -6468,10 +6375,10 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>xydE4Vcj6xU</v>
+        <v>e0WJRMhSrZy</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>If Age is under 18, then warn that Gamaleya is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that AstraZeneca is recommended for ages 18 and up</v>
       </c>
       <c r="C25" s="5" t="str">
         <v/>
@@ -6485,10 +6392,10 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>ppbeGorruVj</v>
+        <v>xydE4Vcj6xU</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>If Age is under 18, then warn that Moderna is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that Gamaleya is recommended for ages 18 and up</v>
       </c>
       <c r="C26" s="4" t="str">
         <v/>
@@ -6502,10 +6409,10 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>xeInMQrA5Mo</v>
+        <v>ppbeGorruVj</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>If Age is under 18, then warn that Sinopharm is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that Moderna is recommended for ages 18 and up</v>
       </c>
       <c r="C27" s="5" t="str">
         <v/>
@@ -6519,10 +6426,10 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>jNtY9t6b120</v>
+        <v>xeInMQrA5Mo</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>if client has a history of cardiovascular disease assign value to current event</v>
+        <v>If Age is under 18, then warn that Sinopharm is recommended for ages 18 and up</v>
       </c>
       <c r="C28" s="4" t="str">
         <v/>
@@ -6536,10 +6443,10 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>j16AULHWXur</v>
+        <v>jNtY9t6b120</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>If client has a history of Cardiovascular disease show it on indicator panel</v>
+        <v>if client has a history of cardiovascular disease assign value to current event</v>
       </c>
       <c r="C29" s="5" t="str">
         <v/>
@@ -6553,10 +6460,10 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>gmBh14b7tYb</v>
+        <v>j16AULHWXur</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>If client has a history of Chronic lung disease show it on indicator panel</v>
+        <v>If client has a history of Cardiovascular disease show it on indicator panel</v>
       </c>
       <c r="C30" s="4" t="str">
         <v/>
@@ -6570,10 +6477,10 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>i0YmXeSnrqn</v>
+        <v>gmBh14b7tYb</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>if client has a history of Chronic lung disease, add value to current event</v>
+        <v>If client has a history of Chronic lung disease show it on indicator panel</v>
       </c>
       <c r="C31" s="5" t="str">
         <v/>
@@ -6587,10 +6494,10 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>KGBdMuY2ASs</v>
+        <v>i0YmXeSnrqn</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>if client has a history of Diabetes assign value to current event</v>
+        <v>if client has a history of Chronic lung disease, add value to current event</v>
       </c>
       <c r="C32" s="4" t="str">
         <v/>
@@ -6604,10 +6511,10 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>r9NQ2R4eFIO</v>
+        <v>KGBdMuY2ASs</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>If client has a history of Diabetes show it on indicator panel</v>
+        <v>if client has a history of Diabetes assign value to current event</v>
       </c>
       <c r="C33" s="5" t="str">
         <v/>
@@ -6621,10 +6528,10 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>i5tOyWRc3S1</v>
+        <v>r9NQ2R4eFIO</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>if client has a history of immunodeficiency assign value to current event</v>
+        <v>If client has a history of Diabetes show it on indicator panel</v>
       </c>
       <c r="C34" s="4" t="str">
         <v/>
@@ -6638,10 +6545,10 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>ucrvgwsRCim</v>
+        <v>i5tOyWRc3S1</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>If client has a history of immunodeficiency show it on indicator panel</v>
+        <v>if client has a history of immunodeficiency assign value to current event</v>
       </c>
       <c r="C35" s="5" t="str">
         <v/>
@@ -6655,10 +6562,10 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>K9Vjkz1xOw1</v>
+        <v>ucrvgwsRCim</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>if client has a history of malignancy assign value to current event</v>
+        <v>If client has a history of immunodeficiency show it on indicator panel</v>
       </c>
       <c r="C36" s="4" t="str">
         <v/>
@@ -6672,10 +6579,10 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>SDfSLD0WFOL</v>
+        <v>K9Vjkz1xOw1</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>if client has a history of malignancy show it on indicator panel</v>
+        <v>if client has a history of malignancy assign value to current event</v>
       </c>
       <c r="C37" s="5" t="str">
         <v/>
@@ -6689,10 +6596,10 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>OdSVYvgu6G2</v>
+        <v>SDfSLD0WFOL</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>if client has a history of neurological deficiency assign value to current event</v>
+        <v>if client has a history of malignancy show it on indicator panel</v>
       </c>
       <c r="C38" s="4" t="str">
         <v/>
@@ -6706,10 +6613,10 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>vqQMyfw3i3u</v>
+        <v>OdSVYvgu6G2</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>If client has a history of Neurological disease show it on indicator panel</v>
+        <v>if client has a history of neurological deficiency assign value to current event</v>
       </c>
       <c r="C39" s="5" t="str">
         <v/>
@@ -6723,10 +6630,10 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>QEq5oRr4UEw</v>
+        <v>vqQMyfw3i3u</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>if client has a history of Other assign value to current event</v>
+        <v>If client has a history of Neurological disease show it on indicator panel</v>
       </c>
       <c r="C40" s="4" t="str">
         <v/>
@@ -6740,10 +6647,10 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="str">
-        <v>ParDbFN1amU</v>
+        <v>QEq5oRr4UEw</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>If client has a history of OTHER disease show it on indicator panel</v>
+        <v>if client has a history of Other assign value to current event</v>
       </c>
       <c r="C41" s="5" t="str">
         <v/>
@@ -6757,10 +6664,10 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>l8opvp32VAd</v>
+        <v>ParDbFN1amU</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>if client has a history of Renal disease assign value to current event</v>
+        <v>If client has a history of OTHER disease show it on indicator panel</v>
       </c>
       <c r="C42" s="4" t="str">
         <v/>
@@ -6774,10 +6681,10 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="str">
-        <v>qrIXRSq77JN</v>
+        <v>l8opvp32VAd</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>If client has a history of Renal Disease show it on indicator panel</v>
+        <v>if client has a history of Renal disease assign value to current event</v>
       </c>
       <c r="C43" s="5" t="str">
         <v/>
@@ -6791,13 +6698,13 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
-        <v>GtxjhHBQdLQ</v>
+        <v>qrIXRSq77JN</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>If patient has had covid, assign value to data element of current event</v>
+        <v>If client has a history of Renal Disease show it on indicator panel</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>Rule transfers date of remission and if person has previously had covid</v>
+        <v/>
       </c>
       <c r="D44" s="4" t="str">
         <v/>
@@ -6808,10 +6715,10 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
-        <v>AmgPexdbztQ</v>
+        <v>GtxjhHBQdLQ</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>If patient has had underlying diseases, transfer that value to following stage</v>
+        <v>If patient has had covid, assign value to data element of current event</v>
       </c>
       <c r="C45" s="5" t="str">
         <v>Rule transfers date of remission and if person has previously had covid</v>
@@ -6825,10 +6732,10 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
-        <v>XTLv9YqOtNX</v>
+        <v>AmgPexdbztQ</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>If previous vaccine is differente than current vaccine, show warning.</v>
+        <v>If patient has had underlying diseases, transfer that value to following stage</v>
       </c>
       <c r="C46" s="4" t="str">
         <v/>
@@ -6842,10 +6749,10 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
-        <v>vd1vZsjDft4</v>
+        <v>XTLv9YqOtNX</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>If previous vaccine is same as current vaccine, hide explanation field</v>
+        <v>If previous vaccine is differente than current vaccine, show warning.</v>
       </c>
       <c r="C47" s="5" t="str">
         <v/>
@@ -6859,10 +6766,10 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
-        <v>A6Oy09dbQwn</v>
+        <v>vd1vZsjDft4</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>if there was an allergic reaction after the first dose, show warning "conduct AEFI Investigation"</v>
+        <v>If previous vaccine is same as current vaccine, hide explanation field</v>
       </c>
       <c r="C48" s="4" t="str">
         <v/>
@@ -6876,13 +6783,13 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="str">
-        <v>PJjKiFrvfuN</v>
+        <v>A6Oy09dbQwn</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>If this is the second dose, mark it as "last dose" for all vaccine products</v>
+        <v>if there was an allergic reaction after the first dose, show warning "conduct AEFI Investigation"</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>It selects the "last dose" option, it assumes that all products have two doses as the complete schedule.</v>
+        <v/>
       </c>
       <c r="D49" s="5" t="str">
         <v/>
@@ -6893,13 +6800,13 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
-        <v>SkBUqyO9zG0</v>
+        <v>PJjKiFrvfuN</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>Last dose - complete programme</v>
+        <v>If this is the second dose, mark it as "last dose" for all vaccine products</v>
       </c>
       <c r="C50" s="4" t="str">
-        <v/>
+        <v>It selects the "last dose" option, it assumes that all products have two doses as the complete schedule.</v>
       </c>
       <c r="D50" s="4" t="str">
         <v/>
@@ -6910,10 +6817,10 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
-        <v>W0YQaz1qRJb</v>
+        <v>SkBUqyO9zG0</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>Send notification if overdue</v>
+        <v>Last dose - complete programme</v>
       </c>
       <c r="C51" s="5" t="str">
         <v/>
@@ -6927,10 +6834,10 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="str">
-        <v>nU9WWRKt7PL</v>
+        <v>W0YQaz1qRJb</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v>Show vaccine type from previous vaccination event</v>
+        <v>Send notification if overdue</v>
       </c>
       <c r="C52" s="4" t="str">
         <v/>
@@ -6944,10 +6851,10 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="str">
-        <v>LO6XtDyCbya</v>
+        <v>nU9WWRKt7PL</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>Show warning if person has had covid within 90 days of vaccination date</v>
+        <v>Show vaccine type from previous vaccination event</v>
       </c>
       <c r="C53" s="5" t="str">
         <v/>
@@ -6961,13 +6868,13 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="str">
-        <v>biYqhZM5HXe</v>
+        <v>LO6XtDyCbya</v>
       </c>
       <c r="B54" s="4" t="str">
-        <v>Show warning if the client is a health worker</v>
+        <v>Show warning if person has had covid within 90 days of vaccination date</v>
       </c>
       <c r="C54" s="4" t="str">
-        <v>If the client is a health worker, show a warning in the top bar</v>
+        <v/>
       </c>
       <c r="D54" s="4" t="str">
         <v/>
@@ -6978,18 +6885,35 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
+        <v>biYqhZM5HXe</v>
+      </c>
+      <c r="B55" s="5" t="str">
+        <v>Show warning if the client is a health worker</v>
+      </c>
+      <c r="C55" s="5" t="str">
+        <v>If the client is a health worker, show a warning in the top bar</v>
+      </c>
+      <c r="D55" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E55" s="5" t="str">
+        <v>yDuAzyqYABS</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="str">
         <v>hdPflHqZKO3</v>
       </c>
-      <c r="B55" s="5" t="str">
+      <c r="B56" s="4" t="str">
         <v>Show warning: If first dose, then hide "last dose" DE</v>
       </c>
-      <c r="C55" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D55" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E55" s="5" t="str">
+      <c r="C56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E56" s="4" t="str">
         <v>yDuAzyqYABS</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add package v1.1.2 for D2.33
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -449,7 +449,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -481,7 +481,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>V1.1.0</v>
+        <v>COVAC</v>
       </c>
     </row>
     <row r="5">
@@ -489,7 +489,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.33.8-3c90b70</v>
+        <v>TRACKER</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>20210302T170052</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="7">
@@ -505,7 +505,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_V1.1.0_DHIS2.33.8-3c90b70_20210302T170052</v>
+        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210318T130229</v>
       </c>
     </row>
   </sheetData>
@@ -582,10 +582,10 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Given name</v>
+        <v>sB1IHYu2xQT</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>TfdH5KvFmMy</v>
+        <v>sB1IHYu2xQT</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
@@ -599,10 +599,10 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Family name</v>
+        <v>ENRjVGxVL6l</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>aW66s2QSosT</v>
+        <v>ENRjVGxVL6l</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
@@ -616,10 +616,10 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Sex</v>
+        <v>oindugucx72</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>CklPZdOd6H1</v>
+        <v>oindugucx72</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
@@ -647,13 +647,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zTWSj3Lg5KP</v>
+        <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Date of birth (age)</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>mAWcalQYYyk</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -670,7 +670,7 @@
         <v>Mobile phone number</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>ciCR6BBvIT4</v>
+        <v>fctSQp5nAYl</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -684,10 +684,10 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Address (current)</v>
+        <v>Xhdn49gUd52</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>VCtm2pySeEV</v>
+        <v>Xhdn49gUd52</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
@@ -781,7 +781,7 @@
         <v>COVAC - AEFIs present</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>AEFIs_present</v>
+        <v>COVAC_AEFIs_present</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>Are there any adverse events present after receiving the immunization?</v>
@@ -1198,7 +1198,7 @@
         <v>totalDoses</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v xml:space="preserve">Total doses required for this vaccine product </v>
+        <v>Total doses required for this vaccine product</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>default</v>
@@ -1258,10 +1258,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
       <c r="C23" s="5" t="str">
         <v>COVAC_vaccine_manufacturer</v>
@@ -1402,7 +1402,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="12">
@@ -1410,7 +1410,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="13">
@@ -1418,7 +1418,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
     <row r="14">
@@ -1426,7 +1426,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="15">
@@ -1434,7 +1434,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="16">
@@ -1442,7 +1442,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="17">
@@ -1450,7 +1450,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="18">
@@ -1458,7 +1458,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="19">
@@ -1466,7 +1466,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="20">
@@ -1474,7 +1474,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="21">
@@ -1482,7 +1482,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="22">
@@ -1490,7 +1490,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="23">
@@ -1506,7 +1506,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1759,7 @@
         <v>kgDmgTYZICP</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>1st Trimester (1-12 weeks); 2nd Trimester (13-28 weeks); 3rd Trimester (20-40 weeks)</v>
+        <v>1st Trimester (1-12 weeks); 2nd Trimester (13-28 weeks); 3rd Trimester (29-40 weeks)</v>
       </c>
     </row>
     <row r="6">
@@ -1806,13 +1806,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Sex</v>
+        <v>Sex</v>
       </c>
       <c r="B9" s="5" t="str">
         <v/>
       </c>
       <c r="C9" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>Female; Male</v>
@@ -1820,13 +1820,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Yes/No/Unknown</v>
+        <v>Yes/No/Unknown</v>
       </c>
       <c r="B10" s="4" t="str">
         <v/>
       </c>
       <c r="C10" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>Yes; No; Unknown</v>
@@ -1957,7 +1957,7 @@
         <v>Q3obJT1MXov</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>3rd Trimester (20-40 weeks)</v>
+        <v>3rd Trimester (29-40 weeks)</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>3trimester</v>
@@ -2090,19 +2090,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>AZK4rjJCss5</v>
+        <v>FKKrOBBFgs1</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>FEMALE</v>
+        <v>Female</v>
       </c>
       <c r="D15" s="5" t="str">
         <v/>
       </c>
       <c r="E15" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
     </row>
     <row r="16">
@@ -2192,19 +2192,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>UrUdMteQzlT</v>
+        <v>Ii4IxCLWEFn</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Male</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>MALE</v>
+        <v>Male</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
       </c>
       <c r="E21" s="5" t="str">
-        <v>hiQ3QFheQ3O</v>
+        <v>WDUwjiW2rGH</v>
       </c>
     </row>
     <row r="22">
@@ -2243,19 +2243,19 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>PLlPgcfbL1D</v>
+        <v>R98tI2c6rF5</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>No</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>NO</v>
+        <v>No</v>
       </c>
       <c r="D24" s="4" t="str">
         <v/>
       </c>
       <c r="E24" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
     <row r="25">
@@ -2515,19 +2515,19 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>TKD1XJ4ZhMO</v>
+        <v>pqxvAQU1z9W</v>
       </c>
       <c r="B40" s="4" t="str">
         <v>Unknown</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>UNKNOWN</v>
+        <v>Unknown</v>
       </c>
       <c r="D40" s="4" t="str">
         <v/>
       </c>
       <c r="E40" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
     <row r="41">
@@ -2549,19 +2549,19 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>CvivP1rh4ii</v>
+        <v>x9yVKkv9koc</v>
       </c>
       <c r="B42" s="4" t="str">
         <v>Yes</v>
       </c>
       <c r="C42" s="4" t="str">
-        <v>YES</v>
+        <v>Yes</v>
       </c>
       <c r="D42" s="4" t="str">
         <v/>
       </c>
       <c r="E42" s="4" t="str">
-        <v>bLA3AqDKdwx</v>
+        <v>L6eMZDJkCwX</v>
       </c>
     </row>
   </sheetData>
@@ -3455,21 +3455,21 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVAC - At least one underlying condition</v>
+        <v>COVAC - People with completed vaccination schedule</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v>COVAC - People with completed vaccination schedule</v>
       </c>
       <c r="C2" s="4" t="str">
         <v/>
       </c>
       <c r="D2" s="4" t="str">
-        <v>gNsB9zivLTy</v>
+        <v>TWG0cq8P539</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVAC - Complete vaccination uptake</v>
+        <v>COVAC - At least one underlying condition</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
@@ -3478,26 +3478,26 @@
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>aUjo2Myd25f</v>
+        <v>gNsB9zivLTy</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
+        <v>COVAC - Underlying conditions</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>TEST TEST</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
       </c>
       <c r="D4" s="4" t="str">
-        <v>vmNUVdhuxN7</v>
+        <v>vFkbMQiABfj</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVAC - Drop-out from COV-1 to COV-c</v>
+        <v>COVAC - Number of doses administered</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
@@ -3506,12 +3506,12 @@
         <v/>
       </c>
       <c r="D5" s="5" t="str">
-        <v>Hbs3xGj7XoN</v>
+        <v>GJPPSQuVt4N</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVAC - Number of doses administered</v>
+        <v>COVAC - Complete vaccination uptake</v>
       </c>
       <c r="B6" s="4" t="str">
         <v xml:space="preserve"> </v>
@@ -3520,26 +3520,26 @@
         <v/>
       </c>
       <c r="D6" s="4" t="str">
-        <v>GJPPSQuVt4N</v>
+        <v>aUjo2Myd25f</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVAC - People with completed vaccination schedule</v>
+        <v>COVAC - Vaccine uptake by sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - People with completed vaccination schedule</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
         <v/>
       </c>
       <c r="D7" s="5" t="str">
-        <v>TWG0cq8P539</v>
+        <v>KV7fffdXnlY</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVAC - Underlying conditions</v>
+        <v>COVAC - Vaccine uptake by age group</v>
       </c>
       <c r="B8" s="4" t="str">
         <v xml:space="preserve"> </v>
@@ -3548,12 +3548,12 @@
         <v/>
       </c>
       <c r="D8" s="4" t="str">
-        <v>vFkbMQiABfj</v>
+        <v>BWlYGFBDbO2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Vaccine uptake by age group</v>
+        <v>COVAC - Vaccine uptake, last month</v>
       </c>
       <c r="B9" s="5" t="str">
         <v xml:space="preserve"> </v>
@@ -3562,12 +3562,12 @@
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>BWlYGFBDbO2</v>
+        <v>MzSAvoJ0vLr</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Vaccine uptake by sex</v>
+        <v>COVAC - Drop-out from COV-1 to COV-c</v>
       </c>
       <c r="B10" s="4" t="str">
         <v xml:space="preserve"> </v>
@@ -3576,21 +3576,21 @@
         <v/>
       </c>
       <c r="D10" s="4" t="str">
-        <v>KV7fffdXnlY</v>
+        <v>Hbs3xGj7XoN</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVAC - Vaccine uptake, last month</v>
+        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>TEST TEST</v>
       </c>
       <c r="C11" s="5" t="str">
         <v/>
       </c>
       <c r="D11" s="5" t="str">
-        <v>MzSAvoJ0vLr</v>
+        <v>vmNUVdhuxN7</v>
       </c>
     </row>
   </sheetData>
@@ -3882,7 +3882,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -3921,14 +3921,6 @@
       </c>
       <c r="B4" s="4" t="str">
         <v>qb8PkSObwqh</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Person</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>loHxNJH4IvV</v>
       </c>
     </row>
   </sheetData>
@@ -4035,14 +4027,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="112.7109375" customWidth="1"/>
+    <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4066,75 +4058,75 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Address (current)</v>
+        <v>Area Urban Rural</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v/>
+        <v>area_urban_rural</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v xml:space="preserve">Current home address of the patient/case </v>
+        <v>Whether client lives in an urban or rural setting</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
       </c>
       <c r="E2" s="4" t="str">
-        <v>VCtm2pySeEV</v>
+        <v>YCqoNJZKvAG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Area Urban Rural</v>
+        <v>COVID - Occupation</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>area_urban_rural</v>
+        <v>occupation</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Whether client lives in an urban or rural setting</v>
+        <v>Client occupation from the pre-defined list</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>YCqoNJZKvAG</v>
+        <v>LY2bDXpNvS7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID - Occupation</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>occupation</v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Client occupation from the pre-defined list</v>
+        <v/>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>LY2bDXpNvS7</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Date of birth (age)</v>
+        <v>Mobile phone number</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Date of birth plus calculated age</v>
+        <v/>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>mAWcalQYYyk</v>
+        <v>fctSQp5nAYl</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>National ID</v>
       </c>
       <c r="B6" s="4" t="str">
         <v/>
@@ -4146,108 +4138,23 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>Ewi7FUfcHAD</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Family name</v>
+        <v>Unique System Identifier (EPI)</v>
       </c>
       <c r="B7" s="5" t="str">
         <v/>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Family name of the patient</v>
+        <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>aW66s2QSosT</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="str">
-        <v>Given name</v>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>The name of the patient or initials</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>TfdH5KvFmMy</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="str">
-        <v>Mobile phone number</v>
-      </c>
-      <c r="B9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>ciCR6BBvIT4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="str">
-        <v>National ID</v>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVAC - Sex</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v>covac_patinfo_sex</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>Sex of Person</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>CklPZdOd6H1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>Unique System Identifier (EPI)</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>System-generated unique ID following pattern: CURRENT_DATE(yyyy-MM-dd) followed by a sequential number (#####)</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4290,7 +4197,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-02</v>
+        <v>2021-03-16</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>
@@ -4329,7 +4236,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>a1jCssI2LkW</v>
@@ -4370,7 +4277,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>Vaccination information</v>
@@ -4381,7 +4288,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Vaccination information</v>
@@ -4392,7 +4299,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Vaccination information</v>
@@ -4403,7 +4310,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Vaccination information</v>
@@ -4414,7 +4321,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Vaccination information</v>
@@ -4425,7 +4332,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B7" s="5" t="str">
         <v>Vaccination information</v>
@@ -4436,7 +4343,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B8" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4447,7 +4354,7 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4458,7 +4365,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B10" s="4" t="str">
         <v>Pre-immunization Questions</v>
@@ -4469,7 +4376,7 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B11" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4480,7 +4387,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4491,7 +4398,7 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B13" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4502,7 +4409,7 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B14" s="4" t="str">
         <v>Pre-immunization Questions</v>
@@ -4513,7 +4420,7 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4524,7 +4431,7 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B16" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4535,7 +4442,7 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B17" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4546,7 +4453,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B18" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4557,7 +4464,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B19" s="5" t="str">
         <v>Underlying Conditions</v>
@@ -4568,7 +4475,7 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B20" s="4" t="str">
         <v>Underlying Conditions</v>
@@ -4579,18 +4486,18 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Vaccination information</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v xml:space="preserve">COVAC - Vaccine Manufacturer </v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B22" s="4" t="str">
         <v>Vaccination information</v>
@@ -4601,7 +4508,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Vaccination information</v>
@@ -4612,7 +4519,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v xml:space="preserve">Vaccination </v>
+        <v>Vaccination</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>Vaccination information</v>
@@ -4985,7 +4892,7 @@
         <v>kNzRGpiCvg4</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v xml:space="preserve">Doses given </v>
+        <v>Doses given</v>
       </c>
       <c r="C14" s="4" t="str">
         <v xml:space="preserve">1st, 2nd, 3rd, booster dose - Number of doses - </v>
@@ -5011,7 +4918,7 @@
         <v>AXweWKC4B3L</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v xml:space="preserve">Number of people receiving a first dose </v>
+        <v>Number of people receiving a first dose</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>First dose - Number of people</v>
@@ -5245,7 +5152,7 @@
         <v>zr25iLoCE4g</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v xml:space="preserve">Number of people receiving a second, third or booster dose </v>
+        <v>Number of people receiving a second, third or booster dose</v>
       </c>
       <c r="C24" s="4" t="str">
         <v>2nd, 3rd, booster dose - Number of people</v>
@@ -5274,7 +5181,7 @@
         <v xml:space="preserve">Number of people receiving a second, third or booster dose  (Male) </v>
       </c>
       <c r="C25" s="5" t="str">
-        <v xml:space="preserve">2nd, 3rd, booster dose - Number of males </v>
+        <v>2nd, 3rd, booster dose - Number of males</v>
       </c>
       <c r="D25" s="5" t="str">
         <v>COV-2 (Male)</v>
@@ -5404,7 +5311,7 @@
         <v xml:space="preserve">Number of people receiving a second, third or booster dose (Female) </v>
       </c>
       <c r="C30" s="4" t="str">
-        <v xml:space="preserve">2nd, 3rd, booster dose - Number of females </v>
+        <v>2nd, 3rd, booster dose - Number of females</v>
       </c>
       <c r="D30" s="4" t="str">
         <v>COV-2 (Female)</v>
@@ -5872,7 +5779,7 @@
         <v>ZZZNumber of doses given</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v xml:space="preserve">ZZZ1st, 2nd, 3rd, booster dose - Number of people </v>
+        <v>ZZZ1st, 2nd, 3rd, booster dose - Number of people</v>
       </c>
       <c r="D48" s="4" t="str">
         <v>ZZZCOV-n</v>
@@ -5895,7 +5802,7 @@
         <v>BEw3zmRnGo4</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v xml:space="preserve">ZZZNumber of people (Female) receiving a second, third or booster dose </v>
+        <v>ZZZNumber of people (Female) receiving a second, third or booster dose</v>
       </c>
       <c r="C49" s="5" t="str">
         <v>ZZZ2nd, 3rd, booster dose - Number of females</v>
@@ -5921,7 +5828,7 @@
         <v>IXW8ahBF3Pl</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v xml:space="preserve">ZZZNumber of people (Male) receiving a second, third or booster dose </v>
+        <v>ZZZNumber of people (Male) receiving a second, third or booster dose</v>
       </c>
       <c r="C50" s="4" t="str">
         <v>ZZZ2nd, 3rd, booster dose - Number of males</v>
@@ -5973,10 +5880,10 @@
         <v>sYIBsws6qUG</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v xml:space="preserve">zzzNumber of people receiving a second, third or booster dose </v>
+        <v>zzzNumber of people receiving a second, third or booster dose</v>
       </c>
       <c r="C52" s="4" t="str">
-        <v xml:space="preserve">zzz2nd, 3rd, booster dose - Number of people </v>
+        <v>zzz2nd, 3rd, booster dose - Number of people</v>
       </c>
       <c r="D52" s="4" t="str">
         <v xml:space="preserve">zzzCOV-2 </v>
@@ -6078,7 +5985,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -6367,7 +6274,7 @@
         <v>oPUB5us9T8e</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v xml:space="preserve">Calculate age </v>
+        <v>Calculate age</v>
       </c>
       <c r="C17" s="5" t="str">
         <v/>
@@ -6432,13 +6339,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>HdOtRsvVzgY</v>
+        <v>R1bzqObecyQ</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Hide Trimester if nor pregnant</v>
+        <v>Hide Suggested date for next dose if vaccine product has no more doses</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v/>
+        <v>All vaccine types with two doses, after they receive one does, the "next dose date" will be hidden.</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
@@ -6449,10 +6356,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>I0FZ4YQgxfD</v>
+        <v>HdOtRsvVzgY</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>Hide underlying conditions if none</v>
+        <v>Hide Trimester if nor pregnant</v>
       </c>
       <c r="C22" s="4" t="str">
         <v/>
@@ -6466,10 +6373,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>TRR2ODBsnkN</v>
+        <v>I0FZ4YQgxfD</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>If Age is under 16, then warn that BioNTech/Pfizer is recommended for ages 16 and up</v>
+        <v>Hide underlying conditions if none</v>
       </c>
       <c r="C23" s="5" t="str">
         <v/>
@@ -6483,10 +6390,10 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>e0WJRMhSrZy</v>
+        <v>TRR2ODBsnkN</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>If Age is under 18, then warn that AstraZeneca is recommended for ages 18 and up</v>
+        <v>If Age is under 16, then warn that BioNTech/Pfizer is recommended for ages 16 and up</v>
       </c>
       <c r="C24" s="4" t="str">
         <v/>
@@ -6500,10 +6407,10 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>xydE4Vcj6xU</v>
+        <v>e0WJRMhSrZy</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>If Age is under 18, then warn that Gamaleya is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that AstraZeneca is recommended for ages 18 and up</v>
       </c>
       <c r="C25" s="5" t="str">
         <v/>
@@ -6517,10 +6424,10 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>ppbeGorruVj</v>
+        <v>xydE4Vcj6xU</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>If Age is under 18, then warn that Moderna is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that Gamaleya is recommended for ages 18 and up</v>
       </c>
       <c r="C26" s="4" t="str">
         <v/>
@@ -6534,10 +6441,10 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>xeInMQrA5Mo</v>
+        <v>ppbeGorruVj</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>If Age is under 18, then warn that Sinopharm is recommended for ages 18 and up</v>
+        <v>If Age is under 18, then warn that Moderna is recommended for ages 18 and up</v>
       </c>
       <c r="C27" s="5" t="str">
         <v/>
@@ -6551,10 +6458,10 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>jNtY9t6b120</v>
+        <v>xeInMQrA5Mo</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>if client has a history of cardiovascular disease assign value to current event</v>
+        <v>If Age is under 18, then warn that Sinopharm is recommended for ages 18 and up</v>
       </c>
       <c r="C28" s="4" t="str">
         <v/>
@@ -6568,10 +6475,10 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>j16AULHWXur</v>
+        <v>jNtY9t6b120</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>If client has a history of Cardiovascular disease show it on indicator panel</v>
+        <v>if client has a history of cardiovascular disease assign value to current event</v>
       </c>
       <c r="C29" s="5" t="str">
         <v/>
@@ -6585,10 +6492,10 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>gmBh14b7tYb</v>
+        <v>j16AULHWXur</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>If client has a history of Chronic lung disease show it on indicator panel</v>
+        <v>If client has a history of Cardiovascular disease show it on indicator panel</v>
       </c>
       <c r="C30" s="4" t="str">
         <v/>
@@ -6602,10 +6509,10 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>i0YmXeSnrqn</v>
+        <v>gmBh14b7tYb</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>if client has a history of Chronic lung disease, add value to current event</v>
+        <v>If client has a history of Chronic lung disease show it on indicator panel</v>
       </c>
       <c r="C31" s="5" t="str">
         <v/>
@@ -6619,10 +6526,10 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>KGBdMuY2ASs</v>
+        <v>i0YmXeSnrqn</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>if client has a history of Diabetes assign value to current event</v>
+        <v>if client has a history of Chronic lung disease, add value to current event</v>
       </c>
       <c r="C32" s="4" t="str">
         <v/>
@@ -6636,10 +6543,10 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>r9NQ2R4eFIO</v>
+        <v>KGBdMuY2ASs</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>If client has a history of Diabetes show it on indicator panel</v>
+        <v>if client has a history of Diabetes assign value to current event</v>
       </c>
       <c r="C33" s="5" t="str">
         <v/>
@@ -6653,10 +6560,10 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>i5tOyWRc3S1</v>
+        <v>r9NQ2R4eFIO</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>if client has a history of immunodeficiency assign value to current event</v>
+        <v>If client has a history of Diabetes show it on indicator panel</v>
       </c>
       <c r="C34" s="4" t="str">
         <v/>
@@ -6670,10 +6577,10 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>ucrvgwsRCim</v>
+        <v>i5tOyWRc3S1</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>If client has a history of immunodeficiency show it on indicator panel</v>
+        <v>if client has a history of immunodeficiency assign value to current event</v>
       </c>
       <c r="C35" s="5" t="str">
         <v/>
@@ -6687,10 +6594,10 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>K9Vjkz1xOw1</v>
+        <v>ucrvgwsRCim</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>if client has a history of malignancy assign value to current event</v>
+        <v>If client has a history of immunodeficiency show it on indicator panel</v>
       </c>
       <c r="C36" s="4" t="str">
         <v/>
@@ -6704,10 +6611,10 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>SDfSLD0WFOL</v>
+        <v>K9Vjkz1xOw1</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>if client has a history of malignancy show it on indicator panel</v>
+        <v>if client has a history of malignancy assign value to current event</v>
       </c>
       <c r="C37" s="5" t="str">
         <v/>
@@ -6721,10 +6628,10 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>OdSVYvgu6G2</v>
+        <v>SDfSLD0WFOL</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>if client has a history of neurological deficiency assign value to current event</v>
+        <v>if client has a history of malignancy show it on indicator panel</v>
       </c>
       <c r="C38" s="4" t="str">
         <v/>
@@ -6738,10 +6645,10 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>vqQMyfw3i3u</v>
+        <v>OdSVYvgu6G2</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>If client has a history of Neurological disease show it on indicator panel</v>
+        <v>if client has a history of neurological deficiency assign value to current event</v>
       </c>
       <c r="C39" s="5" t="str">
         <v/>
@@ -6755,10 +6662,10 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>QEq5oRr4UEw</v>
+        <v>vqQMyfw3i3u</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>if client has a history of Other assign value to current event</v>
+        <v>If client has a history of Neurological disease show it on indicator panel</v>
       </c>
       <c r="C40" s="4" t="str">
         <v/>
@@ -6772,10 +6679,10 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="str">
-        <v>ParDbFN1amU</v>
+        <v>QEq5oRr4UEw</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>If client has a history of OTHER disease show it on indicator panel</v>
+        <v>if client has a history of Other assign value to current event</v>
       </c>
       <c r="C41" s="5" t="str">
         <v/>
@@ -6789,10 +6696,10 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>l8opvp32VAd</v>
+        <v>ParDbFN1amU</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>if client has a history of Renal disease assign value to current event</v>
+        <v>If client has a history of OTHER disease show it on indicator panel</v>
       </c>
       <c r="C42" s="4" t="str">
         <v/>
@@ -6806,10 +6713,10 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="str">
-        <v>qrIXRSq77JN</v>
+        <v>l8opvp32VAd</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>If client has a history of Renal Disease show it on indicator panel</v>
+        <v>if client has a history of Renal disease assign value to current event</v>
       </c>
       <c r="C43" s="5" t="str">
         <v/>
@@ -6823,13 +6730,13 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
-        <v>GtxjhHBQdLQ</v>
+        <v>qrIXRSq77JN</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>If patient has had covid, assign value to data element of current event</v>
+        <v>If client has a history of Renal Disease show it on indicator panel</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>Rule transfers date of remission and if person has previously had covid</v>
+        <v/>
       </c>
       <c r="D44" s="4" t="str">
         <v/>
@@ -6840,10 +6747,10 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
-        <v>AmgPexdbztQ</v>
+        <v>GtxjhHBQdLQ</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>If patient has had underlying diseases, transfer that value to following stage</v>
+        <v>If patient has had covid, assign value to data element of current event</v>
       </c>
       <c r="C45" s="5" t="str">
         <v>Rule transfers date of remission and if person has previously had covid</v>
@@ -6857,10 +6764,10 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
-        <v>XTLv9YqOtNX</v>
+        <v>AmgPexdbztQ</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>If previous vaccine is differente than current vaccine, show warning.</v>
+        <v>If patient has had underlying diseases, transfer that value to following stage</v>
       </c>
       <c r="C46" s="4" t="str">
         <v/>
@@ -6874,10 +6781,10 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
-        <v>vd1vZsjDft4</v>
+        <v>XTLv9YqOtNX</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>If previous vaccine is same as current vaccine, hide explanation field</v>
+        <v>If previous vaccine is differente than current vaccine, show warning.</v>
       </c>
       <c r="C47" s="5" t="str">
         <v/>
@@ -6891,10 +6798,10 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
-        <v>A6Oy09dbQwn</v>
+        <v>vd1vZsjDft4</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>if there was an allergic reaction after the first dose, show warning "conduct AEFI Investigation"</v>
+        <v>If previous vaccine is same as current vaccine, hide explanation field</v>
       </c>
       <c r="C48" s="4" t="str">
         <v/>
@@ -6908,13 +6815,13 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="str">
-        <v>PJjKiFrvfuN</v>
+        <v>A6Oy09dbQwn</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>If this is the second dose, mark it as "last dose" for all vaccine products</v>
+        <v>if there was an allergic reaction after the first dose, show warning "conduct AEFI Investigation"</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>It selects the "last dose" option, it assumes that all products have two doses as the complete schedule.</v>
+        <v/>
       </c>
       <c r="D49" s="5" t="str">
         <v/>
@@ -6925,13 +6832,13 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
-        <v>SkBUqyO9zG0</v>
+        <v>PJjKiFrvfuN</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>Last dose - complete programme</v>
+        <v>If this is the second dose, mark it as "last dose" for all vaccine products</v>
       </c>
       <c r="C50" s="4" t="str">
-        <v/>
+        <v>It selects the "last dose" option, it assumes that all products have two doses as the complete schedule.</v>
       </c>
       <c r="D50" s="4" t="str">
         <v/>
@@ -6942,10 +6849,10 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
-        <v>W0YQaz1qRJb</v>
+        <v>SkBUqyO9zG0</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>Send notification if overdue</v>
+        <v>Last dose - complete programme</v>
       </c>
       <c r="C51" s="5" t="str">
         <v/>
@@ -6959,10 +6866,10 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="str">
-        <v>nU9WWRKt7PL</v>
+        <v>W0YQaz1qRJb</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v>Show vaccine type from previous vaccination event</v>
+        <v>Send notification if overdue</v>
       </c>
       <c r="C52" s="4" t="str">
         <v/>
@@ -6976,10 +6883,10 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="str">
-        <v>LO6XtDyCbya</v>
+        <v>nU9WWRKt7PL</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>Show warning if person has had covid within 90 days of vaccination date</v>
+        <v>Show vaccine type from previous vaccination event</v>
       </c>
       <c r="C53" s="5" t="str">
         <v/>
@@ -6993,13 +6900,13 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="str">
-        <v>biYqhZM5HXe</v>
+        <v>LO6XtDyCbya</v>
       </c>
       <c r="B54" s="4" t="str">
-        <v>Show warning if the client is a health worker</v>
+        <v>Show warning if person has had covid within 90 days of vaccination date</v>
       </c>
       <c r="C54" s="4" t="str">
-        <v>If the client is a health worker, show a warning in the top bar</v>
+        <v/>
       </c>
       <c r="D54" s="4" t="str">
         <v/>
@@ -7010,18 +6917,35 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
+        <v>biYqhZM5HXe</v>
+      </c>
+      <c r="B55" s="5" t="str">
+        <v>Show warning if the client is a health worker</v>
+      </c>
+      <c r="C55" s="5" t="str">
+        <v>If the client is a health worker, show a warning in the top bar</v>
+      </c>
+      <c r="D55" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E55" s="5" t="str">
+        <v>yDuAzyqYABS</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="str">
         <v>hdPflHqZKO3</v>
       </c>
-      <c r="B55" s="5" t="str">
+      <c r="B56" s="4" t="str">
         <v>Show warning: If first dose, then hide "last dose" DE</v>
       </c>
-      <c r="C55" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D55" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E55" s="5" t="str">
+      <c r="C56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E56" s="4" t="str">
         <v>yDuAzyqYABS</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update package for D2.33
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -449,7 +449,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -481,7 +481,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="5">
@@ -489,7 +489,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>TRACKER</v>
+        <v>DHIS2.33.8-3c90b70</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>V1.1.2</v>
+        <v>20210406T115721</v>
       </c>
     </row>
     <row r="7">
@@ -505,7 +505,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210318T130229</v>
+        <v>COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210406T115721</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +582,7 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>sB1IHYu2xQT</v>
+        <v>First Name</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>sB1IHYu2xQT</v>
@@ -599,7 +599,7 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>ENRjVGxVL6l</v>
+        <v>Surname</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>ENRjVGxVL6l</v>
@@ -616,7 +616,7 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>oindugucx72</v>
+        <v>Sex</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>oindugucx72</v>
@@ -650,7 +650,7 @@
         <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>NI0QRzJvQ0k</v>
+        <v>Date of birth</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>NI0QRzJvQ0k</v>
@@ -684,7 +684,7 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Xhdn49gUd52</v>
+        <v>Home Address</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Xhdn49gUd52</v>
@@ -1330,7 +1330,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="3">
@@ -1338,7 +1338,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAC - Underlying condition</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="4">
@@ -1346,7 +1346,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC- Batch Number</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="5">
@@ -1354,7 +1354,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVAC - Pregnancy</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="6">
@@ -1362,7 +1362,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Dose Expiry Date</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="7">
@@ -1370,7 +1370,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Underlying condition</v>
       </c>
     </row>
     <row r="8">
@@ -1378,7 +1378,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - Dose Number</v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="9">
@@ -1386,7 +1386,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVAC - Cardiovascular Disease</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="10">
@@ -1394,7 +1394,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAC - Chronic Lung Disease</v>
+        <v>COVAC- Batch Number</v>
       </c>
     </row>
     <row r="11">
@@ -1402,7 +1402,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="12">
@@ -1410,7 +1410,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="13">
@@ -1418,7 +1418,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="14">
@@ -1426,7 +1426,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC - Pregnancy</v>
       </c>
     </row>
     <row r="15">
@@ -1434,7 +1434,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Dose Expiry Date</v>
       </c>
     </row>
     <row r="16">
@@ -1442,7 +1442,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="17">
@@ -1450,7 +1450,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="18">
@@ -1458,7 +1458,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC - Dose Number</v>
       </c>
     </row>
     <row r="19">
@@ -1466,7 +1466,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC - Malignancy</v>
       </c>
     </row>
     <row r="20">
@@ -1474,7 +1474,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - Cardiovascular Disease</v>
       </c>
     </row>
     <row r="21">
@@ -1482,7 +1482,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Chronic Lung Disease</v>
       </c>
     </row>
     <row r="22">
@@ -1490,7 +1490,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="23">
@@ -1498,7 +1498,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>COVAC - Malignancy</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="24">
@@ -1506,7 +1506,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>COVAC - Vaccine Manufacturer</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
   </sheetData>
@@ -4027,13 +4027,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -4092,10 +4092,10 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>Date of birth</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v/>
+        <v>patinfo_ageonsetunit</v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
@@ -4104,12 +4104,12 @@
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Mobile phone number</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
@@ -4121,15 +4121,15 @@
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>fctSQp5nAYl</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>National ID</v>
+        <v>First Name</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v/>
+        <v>first_name</v>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
@@ -4138,23 +4138,108 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
+        <v>sB1IHYu2xQT</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
+        <v>Home Address</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v>patinfo_resadmin0</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="5" t="str">
+        <v>Xhdn49gUd52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Mobile phone number</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="4" t="str">
+        <v>fctSQp5nAYl</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>National ID</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="5" t="str">
+        <v>Ewi7FUfcHAD</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>Sex</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v>patinfo_sex</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="4" t="str">
+        <v>oindugucx72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>Surname</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v>surname</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>The patient's surname (family name)</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="5" t="str">
+        <v>ENRjVGxVL6l</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
         <v>Unique System Identifier (EPI)</v>
       </c>
-      <c r="B7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C7" s="5" t="str">
+      <c r="B12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C12" s="4" t="str">
         <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
-      <c r="D7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E7" s="5" t="str">
+      <c r="D12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4197,7 +4282,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-16</v>
+        <v>2021-03-19</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>
@@ -4478,10 +4563,10 @@
         <v>Vaccination</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>Underlying Conditions</v>
+        <v>Vaccination information</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="21">
@@ -4489,10 +4574,10 @@
         <v>Vaccination</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Vaccination information</v>
+        <v>Underlying Conditions</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>COVAC - Vaccine Manufacturer</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="22">
@@ -4503,7 +4588,7 @@
         <v>Vaccination information</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="23">
@@ -4514,7 +4599,7 @@
         <v>Vaccination information</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="24">

</xml_diff>

<commit_message>
feat: update package for D2.34
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -26,13 +26,14 @@
     <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
     <sheet name="dashboards" sheetId="22" r:id="rId22"/>
     <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
-    <sheet name="visualizations" sheetId="24" r:id="rId24"/>
-    <sheet name="maps" sheetId="25" r:id="rId25"/>
-    <sheet name="eventCharts" sheetId="26" r:id="rId26"/>
-    <sheet name="trackedEntityInstanceFilters" sheetId="27" r:id="rId27"/>
-    <sheet name="programNotificationTemplates" sheetId="28" r:id="rId28"/>
-    <sheet name="userGroups" sheetId="29" r:id="rId29"/>
-    <sheet name="users" sheetId="30" r:id="rId30"/>
+    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="reportTables" sheetId="25" r:id="rId25"/>
+    <sheet name="maps" sheetId="26" r:id="rId26"/>
+    <sheet name="eventCharts" sheetId="27" r:id="rId27"/>
+    <sheet name="trackedEntityInstanceFilters" sheetId="28" r:id="rId28"/>
+    <sheet name="programNotificationTemplates" sheetId="29" r:id="rId29"/>
+    <sheet name="userGroups" sheetId="30" r:id="rId30"/>
+    <sheet name="users" sheetId="31" r:id="rId31"/>
   </sheets>
 </workbook>
 </file>
@@ -448,7 +449,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,7 +481,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +489,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>TRACKER</v>
+        <v>DHIS2.33.8-3c90b70</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +497,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>V1.1.2</v>
+        <v>20210406T115721</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +505,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.34.3-80c86cc_20210318T014413</v>
+        <v>COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210406T115721</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +582,7 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>sB1IHYu2xQT</v>
+        <v>First Name</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>sB1IHYu2xQT</v>
@@ -598,7 +599,7 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>ENRjVGxVL6l</v>
+        <v>Surname</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>ENRjVGxVL6l</v>
@@ -615,7 +616,7 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>oindugucx72</v>
+        <v>Sex</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>oindugucx72</v>
@@ -649,7 +650,7 @@
         <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>NI0QRzJvQ0k</v>
+        <v>Date of birth</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>NI0QRzJvQ0k</v>
@@ -683,7 +684,7 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Xhdn49gUd52</v>
+        <v>Home Address</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Xhdn49gUd52</v>
@@ -1329,7 +1330,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="3">
@@ -1337,7 +1338,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAC - Underlying condition</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="4">
@@ -1345,7 +1346,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC- Batch Number</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="5">
@@ -1353,7 +1354,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVAC - Pregnancy</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="6">
@@ -1361,7 +1362,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Dose Expiry Date</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="7">
@@ -1369,7 +1370,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Underlying condition</v>
       </c>
     </row>
     <row r="8">
@@ -1377,7 +1378,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - Dose Number</v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="9">
@@ -1385,7 +1386,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVAC - Cardiovascular Disease</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="10">
@@ -1393,7 +1394,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAC - Chronic Lung Disease</v>
+        <v>COVAC- Batch Number</v>
       </c>
     </row>
     <row r="11">
@@ -1401,7 +1402,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="12">
@@ -1409,7 +1410,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="13">
@@ -1417,7 +1418,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="14">
@@ -1425,7 +1426,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC - Pregnancy</v>
       </c>
     </row>
     <row r="15">
@@ -1433,7 +1434,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Dose Expiry Date</v>
       </c>
     </row>
     <row r="16">
@@ -1441,7 +1442,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="17">
@@ -1449,7 +1450,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="18">
@@ -1457,7 +1458,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC - Dose Number</v>
       </c>
     </row>
     <row r="19">
@@ -1465,7 +1466,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC - Malignancy</v>
       </c>
     </row>
     <row r="20">
@@ -1473,7 +1474,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - Cardiovascular Disease</v>
       </c>
     </row>
     <row r="21">
@@ -1481,7 +1482,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Chronic Lung Disease</v>
       </c>
     </row>
     <row r="22">
@@ -1489,7 +1490,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="23">
@@ -1497,7 +1498,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>COVAC - Malignancy</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="24">
@@ -1505,7 +1506,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>COVAC - Vaccine Manufacturer</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
   </sheetData>
@@ -3086,7 +3087,7 @@
         <v>TWG0cq8P539</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>SINGLE_VALUE</v>
+        <v>Chart</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>COVAC - People with completed vaccination schedule</v>
@@ -3186,7 +3187,7 @@
         <v>wHd33PaphEC</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>PIVOT_TABLE</v>
+        <v>Pivot table</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
@@ -3206,7 +3207,7 @@
         <v>gNsB9zivLTy</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COLUMN</v>
+        <v>Chart</v>
       </c>
       <c r="C11" s="5" t="str">
         <v>COVAC - At least one underlying condition</v>
@@ -3226,7 +3227,7 @@
         <v>vFkbMQiABfj</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>PIE</v>
+        <v>Chart</v>
       </c>
       <c r="C12" s="4" t="str">
         <v>COVAC - Underlying conditions</v>
@@ -3243,13 +3244,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v/>
+        <v>Db3MWC56CBp</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>MAP</v>
+        <v>Map</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v/>
+        <v>COVAC-Dropout rates</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>XaeVdRGnR7J</v>
@@ -3266,7 +3267,7 @@
         <v>GJPPSQuVt4N</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>SINGLE_VALUE</v>
+        <v>Chart</v>
       </c>
       <c r="C14" s="4" t="str">
         <v>COVAC - Number of doses administered</v>
@@ -3286,7 +3287,7 @@
         <v>aUjo2Myd25f</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COLUMN</v>
+        <v>Chart</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>COVAC - Complete vaccination uptake</v>
@@ -3306,7 +3307,7 @@
         <v>KV7fffdXnlY</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>PIE</v>
+        <v>Chart</v>
       </c>
       <c r="C16" s="4" t="str">
         <v>COVAC - Vaccine uptake by sex</v>
@@ -3326,7 +3327,7 @@
         <v>BWlYGFBDbO2</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>PIE</v>
+        <v>Chart</v>
       </c>
       <c r="C17" s="5" t="str">
         <v>COVAC - Vaccine uptake by age group</v>
@@ -3346,7 +3347,7 @@
         <v>MzSAvoJ0vLr</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>PIE</v>
+        <v>Chart</v>
       </c>
       <c r="C18" s="4" t="str">
         <v>COVAC - Vaccine uptake, last month</v>
@@ -3363,13 +3364,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v/>
+        <v>cOH1OjReS14</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>MAP</v>
+        <v>Map</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v/>
+        <v>COVAC-Number of doses given, last month</v>
       </c>
       <c r="D19" s="5" t="str">
         <v>BKU0qpNqRJt</v>
@@ -3386,7 +3387,7 @@
         <v>Hbs3xGj7XoN</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>LINE</v>
+        <v>Chart</v>
       </c>
       <c r="C20" s="4" t="str">
         <v>COVAC - Drop-out from COV-1 to COV-c</v>
@@ -3406,7 +3407,7 @@
         <v>vmNUVdhuxN7</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>STACKED_COLUMN</v>
+        <v>Chart</v>
       </c>
       <c r="C21" s="5" t="str">
         <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
@@ -3427,12 +3428,12 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="86.7109375" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
     <col min="2" max="2" width="52.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -3468,141 +3469,127 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
+        <v>COVAC - At least one underlying condition</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>wHd33PaphEC</v>
+        <v>gNsB9zivLTy</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVAC - At least one underlying condition</v>
+        <v>COVAC - Underlying conditions</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
       </c>
       <c r="D4" s="4" t="str">
-        <v>gNsB9zivLTy</v>
+        <v>vFkbMQiABfj</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVAC - Underlying conditions</v>
+        <v>COVAC - Number of doses administered</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
         <v/>
       </c>
       <c r="D5" s="5" t="str">
-        <v>vFkbMQiABfj</v>
+        <v>GJPPSQuVt4N</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVAC - Number of doses administered</v>
+        <v>COVAC - Complete vaccination uptake</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
       </c>
       <c r="D6" s="4" t="str">
-        <v>GJPPSQuVt4N</v>
+        <v>aUjo2Myd25f</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVAC - Complete vaccination uptake</v>
+        <v>COVAC - Vaccine uptake by sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
         <v/>
       </c>
       <c r="D7" s="5" t="str">
-        <v>aUjo2Myd25f</v>
+        <v>KV7fffdXnlY</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVAC - Vaccine uptake by sex</v>
+        <v>COVAC - Vaccine uptake by age group</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
         <v/>
       </c>
       <c r="D8" s="4" t="str">
-        <v>KV7fffdXnlY</v>
+        <v>BWlYGFBDbO2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Vaccine uptake by age group</v>
+        <v>COVAC - Vaccine uptake, last month</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>BWlYGFBDbO2</v>
+        <v>MzSAvoJ0vLr</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Vaccine uptake, last month</v>
+        <v>COVAC - Drop-out from COV-1 to COV-c</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
         <v/>
       </c>
       <c r="D10" s="4" t="str">
-        <v>MzSAvoJ0vLr</v>
+        <v>Hbs3xGj7XoN</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVAC - Drop-out from COV-1 to COV-c</v>
+        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v/>
+        <v>TEST TEST</v>
       </c>
       <c r="C11" s="5" t="str">
         <v/>
       </c>
       <c r="D11" s="5" t="str">
-        <v>Hbs3xGj7XoN</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v>TEST TEST</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D12" s="4" t="str">
         <v>vmNUVdhuxN7</v>
       </c>
     </row>
@@ -3611,6 +3598,51 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="86.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>wHd33PaphEC</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3669,7 +3701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3728,7 +3760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3799,7 +3831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3842,66 +3874,6 @@
       </c>
       <c r="C3" s="5" t="str">
         <v/>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVAC - Covid-19 Immunization Data Analysis</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>VLIaHu6ou8E</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVAC - Covid-19 Immunization Data Entry</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>q3Nh5xhJEy2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVAC - Covid-19 Immunization Metadata Admin</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>AEAQ9LktNze</v>
       </c>
     </row>
   </sheetData>
@@ -3957,6 +3929,66 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVAC - Covid-19 Immunization Data Analysis</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>VLIaHu6ou8E</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVAC - Covid-19 Immunization Data Entry</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>q3Nh5xhJEy2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>COVAC - Covid-19 Immunization Metadata Admin</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>AEAQ9LktNze</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
@@ -3995,13 +4027,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -4060,10 +4092,10 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>Date of birth</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v/>
+        <v>patinfo_ageonsetunit</v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
@@ -4072,12 +4104,12 @@
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Mobile phone number</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
@@ -4089,15 +4121,15 @@
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>fctSQp5nAYl</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>National ID</v>
+        <v>First Name</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v/>
+        <v>first_name</v>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
@@ -4106,23 +4138,108 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
+        <v>sB1IHYu2xQT</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
+        <v>Home Address</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v>patinfo_resadmin0</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="5" t="str">
+        <v>Xhdn49gUd52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Mobile phone number</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="4" t="str">
+        <v>fctSQp5nAYl</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>National ID</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="5" t="str">
+        <v>Ewi7FUfcHAD</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>Sex</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v>patinfo_sex</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="4" t="str">
+        <v>oindugucx72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>Surname</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v>surname</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>The patient's surname (family name)</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="5" t="str">
+        <v>ENRjVGxVL6l</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
         <v>Unique System Identifier (EPI)</v>
       </c>
-      <c r="B7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C7" s="5" t="str">
+      <c r="B12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C12" s="4" t="str">
         <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
-      <c r="D7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E7" s="5" t="str">
+      <c r="D12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4165,7 +4282,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-16</v>
+        <v>2021-03-19</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>

</xml_diff>

<commit_message>
feat: update package for D2.35
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -448,7 +448,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,7 +480,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +488,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>TRACKER</v>
+        <v>DHIS2.35.3-3492688</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>V1.1.2</v>
+        <v>20210408T081801</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.35.1-bca7d7b_20210318T015424</v>
+        <v>COVAC_TRACKER_V1.1.2_DHIS2.35.3-3492688_20210408T081801</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +581,7 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>sB1IHYu2xQT</v>
+        <v>First Name</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>sB1IHYu2xQT</v>
@@ -598,7 +598,7 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>ENRjVGxVL6l</v>
+        <v>Surname</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>ENRjVGxVL6l</v>
@@ -615,7 +615,7 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>oindugucx72</v>
+        <v>Sex</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>oindugucx72</v>
@@ -649,7 +649,7 @@
         <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>NI0QRzJvQ0k</v>
+        <v>Date of birth</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>NI0QRzJvQ0k</v>
@@ -683,7 +683,7 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Xhdn49gUd52</v>
+        <v>Home Address</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Xhdn49gUd52</v>
@@ -1337,7 +1337,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAC - Dose Number</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="4">
@@ -1345,7 +1345,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Dose Number</v>
       </c>
     </row>
     <row r="5">
@@ -1353,7 +1353,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC- Batch Number</v>
       </c>
     </row>
     <row r="6">
@@ -1361,7 +1361,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Pregnancy</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="7">
@@ -1369,7 +1369,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Malignancy</v>
       </c>
     </row>
     <row r="8">
@@ -1377,7 +1377,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="9">
@@ -1385,7 +1385,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Pregnancy</v>
       </c>
     </row>
     <row r="10">
@@ -1393,7 +1393,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="11">
@@ -1401,7 +1401,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
     <row r="12">
@@ -1409,7 +1409,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="13">
@@ -1417,7 +1417,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="14">
@@ -1425,7 +1425,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC - Vaccine Manufacturer</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="15">
@@ -1433,7 +1433,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC- Batch Number</v>
+        <v>COVAC - Cardiovascular Disease</v>
       </c>
     </row>
     <row r="16">
@@ -1441,7 +1441,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Malignancy</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="17">
@@ -1449,7 +1449,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="18">
@@ -1457,7 +1457,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="19">
@@ -1465,7 +1465,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="20">
@@ -1473,7 +1473,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Cardiovascular Disease</v>
+        <v>COVAC - Chronic Lung Disease</v>
       </c>
     </row>
     <row r="21">
@@ -1481,7 +1481,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="22">
@@ -1489,7 +1489,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC - Chronic Lung Disease</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="23">
@@ -1497,7 +1497,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Underlying condition</v>
       </c>
     </row>
     <row r="24">
@@ -1505,7 +1505,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>COVAC - Underlying condition</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
   </sheetData>
@@ -3995,13 +3995,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -4060,10 +4060,10 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>Date of birth</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v/>
+        <v>patinfo_ageonsetunit</v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
@@ -4072,12 +4072,12 @@
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Mobile phone number</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
@@ -4089,15 +4089,15 @@
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>fctSQp5nAYl</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>National ID</v>
+        <v>First Name</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v/>
+        <v>first_name</v>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
@@ -4106,23 +4106,108 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
+        <v>sB1IHYu2xQT</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
+        <v>Home Address</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v>patinfo_resadmin0</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="5" t="str">
+        <v>Xhdn49gUd52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Mobile phone number</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="4" t="str">
+        <v>fctSQp5nAYl</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>National ID</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="5" t="str">
+        <v>Ewi7FUfcHAD</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>Sex</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v>patinfo_sex</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="4" t="str">
+        <v>oindugucx72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>Surname</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v>surname</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>The patient's surname (family name)</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="5" t="str">
+        <v>ENRjVGxVL6l</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
         <v>Unique System Identifier (EPI)</v>
       </c>
-      <c r="B7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C7" s="5" t="str">
+      <c r="B12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C12" s="4" t="str">
         <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
-      <c r="D7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E7" s="5" t="str">
+      <c r="D12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4165,7 +4250,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-16</v>
+        <v>2021-03-19</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>

</xml_diff>

<commit_message>
fix: replace metadata with correct file
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -26,14 +26,13 @@
     <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
     <sheet name="dashboards" sheetId="22" r:id="rId22"/>
     <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
-    <sheet name="charts" sheetId="24" r:id="rId24"/>
-    <sheet name="reportTables" sheetId="25" r:id="rId25"/>
-    <sheet name="maps" sheetId="26" r:id="rId26"/>
-    <sheet name="eventCharts" sheetId="27" r:id="rId27"/>
-    <sheet name="trackedEntityInstanceFilters" sheetId="28" r:id="rId28"/>
-    <sheet name="programNotificationTemplates" sheetId="29" r:id="rId29"/>
-    <sheet name="userGroups" sheetId="30" r:id="rId30"/>
-    <sheet name="users" sheetId="31" r:id="rId31"/>
+    <sheet name="visualizations" sheetId="24" r:id="rId24"/>
+    <sheet name="maps" sheetId="25" r:id="rId25"/>
+    <sheet name="eventCharts" sheetId="26" r:id="rId26"/>
+    <sheet name="trackedEntityInstanceFilters" sheetId="27" r:id="rId27"/>
+    <sheet name="programNotificationTemplates" sheetId="28" r:id="rId28"/>
+    <sheet name="userGroups" sheetId="29" r:id="rId29"/>
+    <sheet name="users" sheetId="30" r:id="rId30"/>
   </sheets>
 </workbook>
 </file>
@@ -489,7 +488,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.33.8-3c90b70</v>
+        <v>DHIS2.34.4-aff07fb</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +496,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>20210406T115721</v>
+        <v>20210406T141800</v>
       </c>
     </row>
     <row r="7">
@@ -505,7 +504,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210406T115721</v>
+        <v>COVAC_TRACKER_V1.1.2_DHIS2.34.4-aff07fb_20210406T141800</v>
       </c>
     </row>
   </sheetData>
@@ -3087,7 +3086,7 @@
         <v>TWG0cq8P539</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>COVAC - People with completed vaccination schedule</v>
@@ -3187,7 +3186,7 @@
         <v>wHd33PaphEC</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Pivot table</v>
+        <v>PIVOT_TABLE</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
@@ -3207,7 +3206,7 @@
         <v>gNsB9zivLTy</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C11" s="5" t="str">
         <v>COVAC - At least one underlying condition</v>
@@ -3227,7 +3226,7 @@
         <v>vFkbMQiABfj</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C12" s="4" t="str">
         <v>COVAC - Underlying conditions</v>
@@ -3244,13 +3243,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>Db3MWC56CBp</v>
+        <v/>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Map</v>
+        <v>MAP</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>COVAC-Dropout rates</v>
+        <v/>
       </c>
       <c r="D13" s="5" t="str">
         <v>XaeVdRGnR7J</v>
@@ -3267,7 +3266,7 @@
         <v>GJPPSQuVt4N</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Chart</v>
+        <v>SINGLE_VALUE</v>
       </c>
       <c r="C14" s="4" t="str">
         <v>COVAC - Number of doses administered</v>
@@ -3287,7 +3286,7 @@
         <v>aUjo2Myd25f</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Chart</v>
+        <v>COLUMN</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>COVAC - Complete vaccination uptake</v>
@@ -3307,7 +3306,7 @@
         <v>KV7fffdXnlY</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C16" s="4" t="str">
         <v>COVAC - Vaccine uptake by sex</v>
@@ -3327,7 +3326,7 @@
         <v>BWlYGFBDbO2</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C17" s="5" t="str">
         <v>COVAC - Vaccine uptake by age group</v>
@@ -3347,7 +3346,7 @@
         <v>MzSAvoJ0vLr</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Chart</v>
+        <v>PIE</v>
       </c>
       <c r="C18" s="4" t="str">
         <v>COVAC - Vaccine uptake, last month</v>
@@ -3364,13 +3363,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>cOH1OjReS14</v>
+        <v/>
       </c>
       <c r="B19" s="5" t="str">
-        <v>Map</v>
+        <v>MAP</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>COVAC-Number of doses given, last month</v>
+        <v/>
       </c>
       <c r="D19" s="5" t="str">
         <v>BKU0qpNqRJt</v>
@@ -3387,7 +3386,7 @@
         <v>Hbs3xGj7XoN</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>Chart</v>
+        <v>LINE</v>
       </c>
       <c r="C20" s="4" t="str">
         <v>COVAC - Drop-out from COV-1 to COV-c</v>
@@ -3407,7 +3406,7 @@
         <v>vmNUVdhuxN7</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Chart</v>
+        <v>STACKED_COLUMN</v>
       </c>
       <c r="C21" s="5" t="str">
         <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
@@ -3428,12 +3427,12 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="86.7109375" customWidth="1"/>
     <col min="2" max="2" width="52.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -3469,127 +3468,141 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVAC - At least one underlying condition</v>
+        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C3" s="5" t="str">
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>gNsB9zivLTy</v>
+        <v>wHd33PaphEC</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVAC - Underlying conditions</v>
+        <v>COVAC - At least one underlying condition</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
       </c>
       <c r="D4" s="4" t="str">
-        <v>vFkbMQiABfj</v>
+        <v>gNsB9zivLTy</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVAC - Number of doses administered</v>
+        <v>COVAC - Underlying conditions</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C5" s="5" t="str">
         <v/>
       </c>
       <c r="D5" s="5" t="str">
-        <v>GJPPSQuVt4N</v>
+        <v>vFkbMQiABfj</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVAC - Complete vaccination uptake</v>
+        <v>COVAC - Number of doses administered</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
       </c>
       <c r="D6" s="4" t="str">
-        <v>aUjo2Myd25f</v>
+        <v>GJPPSQuVt4N</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVAC - Vaccine uptake by sex</v>
+        <v>COVAC - Complete vaccination uptake</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C7" s="5" t="str">
         <v/>
       </c>
       <c r="D7" s="5" t="str">
-        <v>KV7fffdXnlY</v>
+        <v>aUjo2Myd25f</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVAC - Vaccine uptake by age group</v>
+        <v>COVAC - Vaccine uptake by sex</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C8" s="4" t="str">
         <v/>
       </c>
       <c r="D8" s="4" t="str">
-        <v>BWlYGFBDbO2</v>
+        <v>KV7fffdXnlY</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVAC - Vaccine uptake, last month</v>
+        <v>COVAC - Vaccine uptake by age group</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C9" s="5" t="str">
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>MzSAvoJ0vLr</v>
+        <v>BWlYGFBDbO2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAC - Drop-out from COV-1 to COV-c</v>
+        <v>COVAC - Vaccine uptake, last month</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
       <c r="C10" s="4" t="str">
         <v/>
       </c>
       <c r="D10" s="4" t="str">
-        <v>Hbs3xGj7XoN</v>
+        <v>MzSAvoJ0vLr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
+        <v>COVAC - Drop-out from COV-1 to COV-c</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v>Hbs3xGj7XoN</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
         <v>COVAC - Cumulative number of given doses, Last 4 weeks</v>
       </c>
-      <c r="B11" s="5" t="str">
+      <c r="B12" s="4" t="str">
         <v>TEST TEST</v>
       </c>
-      <c r="C11" s="5" t="str">
-        <v/>
-      </c>
-      <c r="D11" s="5" t="str">
+      <c r="C12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D12" s="4" t="str">
         <v>vmNUVdhuxN7</v>
       </c>
     </row>
@@ -3598,51 +3611,6 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="86.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVAC - People receiving COV-2 vs People completing the vaccination schedule (Cov-C)</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>wHd33PaphEC</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3701,7 +3669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3760,7 +3728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3831,7 +3799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3874,6 +3842,66 @@
       </c>
       <c r="C3" s="5" t="str">
         <v/>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVAC - Covid-19 Immunization Data Analysis</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>VLIaHu6ou8E</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVAC - Covid-19 Immunization Data Entry</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>q3Nh5xhJEy2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>COVAC - Covid-19 Immunization Metadata Admin</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>AEAQ9LktNze</v>
       </c>
     </row>
   </sheetData>
@@ -3928,66 +3956,6 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVAC - Covid-19 Immunization Data Analysis</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>VLIaHu6ou8E</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVAC - Covid-19 Immunization Data Entry</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>q3Nh5xhJEy2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVAC - Covid-19 Immunization Metadata Admin</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>AEAQ9LktNze</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4282,7 +4250,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-19</v>
+        <v>2021-04-06</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>

</xml_diff>